<commit_message>
Replaced heritage pics w/ illustrations
</commit_message>
<xml_diff>
--- a/src/data/workshop_data/recommended_books.xlsx
+++ b/src/data/workshop_data/recommended_books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\workshop_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F3A463-733E-4343-A7FE-DDBB3D244500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECF7F38-6D53-489E-A335-EF6B91C31F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{BE54A3D7-AD18-4D3A-9B07-972BEB6CC897}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$250</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$N$265</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="1354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="1393">
   <si>
     <t>recommender</t>
   </si>
@@ -4320,6 +4320,130 @@
   <si>
     <t>TPM</t>
   </si>
+  <si>
+    <t>Capital in the Twenty-First Century</t>
+  </si>
+  <si>
+    <t>Thomas Piketty</t>
+  </si>
+  <si>
+    <t>978-0674430006</t>
+  </si>
+  <si>
+    <t>What are the grand dynamics that drive the accumulation and distribution of capital? Questions about the long-term evolution of inequality, the concentration of wealth, and the prospects for economic growth lie at the heart of political economy. But satisfactory answers have been hard to find for lack of adequate data and clear guiding theories. In this work the author analyzes a unique collection of data from twenty countries, ranging as far back as the eighteenth century, to uncover key economic and social patterns. His findings transform debate and set the agenda for the next generation of thought about wealth and inequality. He shows that modern economic growth and the diffusion of knowledge have allowed us to avoid inequalities on the apocalyptic scale predicted by Karl Marx. But we have not modified the deep structures of capital and inequality as much as we thought in the optimistic decades following World War II. The main driver of inequality--the tendency of returns on capital to exceed the rate of economic growth--today threatens to generate extreme inequalities that stir discontent and undermine democratic values if political action is not taken. But economic trends are not acts of God. Political action has curbed dangerous inequalities in the past, the author says, and may do so again. This original work reorients our understanding of economic history and confronts us with sobering lessons for today.</t>
+  </si>
+  <si>
+    <t>858914389.webp</t>
+  </si>
+  <si>
+    <t>Abstract Art</t>
+  </si>
+  <si>
+    <t>Dietmar Elger</t>
+  </si>
+  <si>
+    <t>978-3836546782</t>
+  </si>
+  <si>
+    <t>A survey of abstract art and its influences on the 20th century art scene."This essential introduction spans the international breadth, conceptual depth, and seismic impact of abstract art with a thorough survey not only of the big names such as Picasso, Klee, Kline, Rothko, and Pollock, but also lesser-known figures who made equally significant contributions, including Antoni Tàpies, K.O. Götz, Ad Reinhardt, and Sophie Taeuber-Arp.</t>
+  </si>
+  <si>
+    <t>1379313397.webp</t>
+  </si>
+  <si>
+    <t>Vision Science: Photons to Phenomenology</t>
+  </si>
+  <si>
+    <t>978-0262161831</t>
+  </si>
+  <si>
+    <t>Stephen E Palmer</t>
+  </si>
+  <si>
+    <t>782888043.webp</t>
+  </si>
+  <si>
+    <t>This book revolutionizes how vision can be taught to undergraduate and graduate students in cognitive science, psychology, and optometry. It is the first comprehensive textbook on vision to reflect the integrated computational approach of modern research scientists. This new interdisciplinary approach, called "vision science," integrates psychological, computational, and neuroscientific perspectives.
+The book covers all major topics related to vision, from early neural processing of image structure in the retina to high-level visual attention, memory, imagery, and awareness. The presentation throughout is theoretically sophisticated yet requires minimal knowledge of mathematics. There is also an extensive glossary, as well as appendices on psychophysical methods, connectionist modeling, and color technology. The book will serve not only as a comprehensive textbook on vision, but also as a valuable reference for researchers in cognitive science, psychology, neuroscience, computer science, optometry, and philosophy.</t>
+  </si>
+  <si>
+    <t>The fundamentals of sonic art &amp; sound design</t>
+  </si>
+  <si>
+    <t>978-2940373499</t>
+  </si>
+  <si>
+    <t>Tony Gibbs</t>
+  </si>
+  <si>
+    <t>82672512.webp</t>
+  </si>
+  <si>
+    <t>This book introduces a subject that will be new to many: sonic arts. The application of sound to other media (such as film or video) is well known and the idea of sound as a medium in its own right (such as radio) is also widely accepted. However, the idea that sound could also be a distinct art form by itself is less well established and often misunderstood. The Fundamentals of Sonic Arts &amp; Sound Design introduces, describes and begins the process of defining this new subject and to provide a starting point for anyone who has an interest in the creative uses of sound. The book explores the worlds of sonic arts and sound design through their history and development, and looks at the present state of these extraordinarily diverse genres through the works and words of established artists and through an examination of the wide range of practices that currently come under the heading of sonic arts. The technologies that are used and the impact that they have upon the work are also discussed. Additionally, The Fundamentals of Sonic Arts &amp; Sound Design considers new and radical approaches to sound recording, performance, installation works and exhibitions and visits the worlds of the sonic artist and the sound designer.</t>
+  </si>
+  <si>
+    <t>Foundations in sound design for embedded media: a multidisciplinary approach</t>
+  </si>
+  <si>
+    <t>978-1138093874</t>
+  </si>
+  <si>
+    <t>Michael Filimowicz</t>
+  </si>
+  <si>
+    <t>1086015792.webp</t>
+  </si>
+  <si>
+    <t>This volume provides a comprehensive introduction to foundational topics in sound design for embedded media, such as physical computing; interaction design; auditory displays and data sonification; speech synthesis; wearables; smart objects and instruments; user experience; toys and playful tangible objects; and the new sensibilities entailed in expanding the concept of sound design to encompass the totality of our surroundings. The reader will gain a broad understanding of the key concepts and practices that define sound design for its use in computational products and design. The chapters are written by international authors from diverse backgrounds who provide multidisciplinary perspectives on sound in its many embedded forms. The volume is designed as a textbook for students and teachers, as a handbook for researchers in sound, programming and design, and as a survey of key trends and ideas for practitioners interested in exploring the boundaries of their profession.</t>
+  </si>
+  <si>
+    <t>The Art of Perception: Mastering the Gestalt Principles of Visual Organization</t>
+  </si>
+  <si>
+    <t>Light for Visual Artists: Understanding and Using Light in Art &amp; Design</t>
+  </si>
+  <si>
+    <t>Archeologies of Touch</t>
+  </si>
+  <si>
+    <t>The Touch: Spaces Designed for the Senses</t>
+  </si>
+  <si>
+    <t>Strange Tools</t>
+  </si>
+  <si>
+    <t>Ways of Seeing</t>
+  </si>
+  <si>
+    <t>Sound and Image: Aesthetics and Practices</t>
+  </si>
+  <si>
+    <t>Eyes of the Skin</t>
+  </si>
+  <si>
+    <t>Synesthetic Design: Handbook for a Multi-Sensory Approach</t>
+  </si>
+  <si>
+    <t>Ferdy Saitta</t>
+  </si>
+  <si>
+    <t>Are you struggling to create visually captivating designs that resonate with your audience? Do you find it challenging to organize and communicate your visual ideas effectively? Look no further, as "The Art of Perception: Mastering the Gestalt Principles of Visual Organization" is here to solve your design dilemmas.
+In this groundbreaking book, we unravel the secrets of visual organization and perception, providing you with a comprehensive toolkit to transform your design approach. No more guesswork or trial and error. We offer you a clear path to mastering the Gestalt Principles, the fundamental building blocks of visual communication.
+Have you ever wondered why certain designs instantly catch your eye, and others go unnoticed? Our book reveals the answer by diving deep into each Gestalt Principle, breaking them into simple, actionable insights. You'll gain a profound understanding of how the human mind perceives and processes visual information, enabling you to create designs that engage, inspire, and leave a lasting impact.
+"The Art of Perception" is not just another theoretical guide. It's a hands-on resource with practical examples and real-world case studies. You'll witness the power of the Gestalt Principles firsthand as you apply them to your design projects. From graphic design and branding to user experience and motion design, we provide practical applications for various fields, equipping you with the tools to elevate your work across industries.
+Gone are the days of designing in the dark, hoping for the best. Our book empowers you to make informed design decisions based on solid principles and proven techniques.
+Whether you're a seasoned designer looking to enhance your skills or a novice seeking to understand the foundations of visual communication, "The Art of Perception" is your roadmap to success. It's time to unleash the true potential of your designs, captivate your audience, and stand out in a visually cluttered world.
+Don't let your designs go unnoticed or fall short of their intended impact. Grab your copy of "The Art of Perception: Mastering the Gestalt Principles of Visual Organization" on Amazon Kindle today and embark on a transformative journey that will forever change the way you approach design. Say goodbye to design challenges and hello to captivating, visually organized creations that leave a lasting impression.</t>
+  </si>
+  <si>
+    <t>978-XXXXXXXXXX</t>
+  </si>
+  <si>
+    <t>71Xo87sjRJL</t>
+  </si>
+  <si>
+    <t>71Xo87sjRJL.webp</t>
+  </si>
 </sst>
 </file>
 
@@ -4398,7 +4522,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4412,6 +4536,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4746,10 +4871,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17C54CB-A494-4D8A-8C6C-09250B011A75}">
-  <dimension ref="A1:N250"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N265"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E254" sqref="E254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4811,7 +4937,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>435</v>
       </c>
@@ -4834,7 +4960,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>435</v>
       </c>
@@ -4857,7 +4983,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>132</v>
       </c>
@@ -4898,7 +5024,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -4939,7 +5065,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>378</v>
       </c>
@@ -4980,7 +5106,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>154</v>
       </c>
@@ -5021,7 +5147,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>175</v>
       </c>
@@ -5062,7 +5188,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>420</v>
       </c>
@@ -5103,7 +5229,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>446</v>
       </c>
@@ -5144,7 +5270,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -5185,7 +5311,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>289</v>
       </c>
@@ -5226,7 +5352,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>435</v>
       </c>
@@ -5249,7 +5375,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -5290,7 +5416,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>339</v>
       </c>
@@ -5331,7 +5457,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>88</v>
       </c>
@@ -5372,7 +5498,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>435</v>
       </c>
@@ -5395,7 +5521,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>435</v>
       </c>
@@ -5418,7 +5544,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>271</v>
       </c>
@@ -5459,7 +5585,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>339</v>
       </c>
@@ -5500,7 +5626,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>361</v>
       </c>
@@ -5541,7 +5667,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>154</v>
       </c>
@@ -5582,7 +5708,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>435</v>
       </c>
@@ -5605,7 +5731,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>175</v>
       </c>
@@ -5646,7 +5772,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>300</v>
       </c>
@@ -5687,7 +5813,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>435</v>
       </c>
@@ -5710,7 +5836,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>271</v>
       </c>
@@ -5751,7 +5877,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>361</v>
       </c>
@@ -5792,7 +5918,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>435</v>
       </c>
@@ -5815,7 +5941,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>435</v>
       </c>
@@ -5838,7 +5964,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -5879,7 +6005,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>69</v>
       </c>
@@ -5920,7 +6046,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -5961,7 +6087,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>212</v>
       </c>
@@ -6002,7 +6128,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>420</v>
       </c>
@@ -6043,7 +6169,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>271</v>
       </c>
@@ -6084,7 +6210,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -6125,7 +6251,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>435</v>
       </c>
@@ -6148,7 +6274,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>339</v>
       </c>
@@ -6189,7 +6315,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>190</v>
       </c>
@@ -6230,7 +6356,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>110</v>
       </c>
@@ -6271,7 +6397,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>398</v>
       </c>
@@ -6312,7 +6438,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>361</v>
       </c>
@@ -6353,7 +6479,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>300</v>
       </c>
@@ -6394,7 +6520,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>318</v>
       </c>
@@ -6435,7 +6561,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>318</v>
       </c>
@@ -6476,7 +6602,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>398</v>
       </c>
@@ -6517,7 +6643,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>420</v>
       </c>
@@ -6558,7 +6684,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>190</v>
       </c>
@@ -6599,7 +6725,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>398</v>
       </c>
@@ -6640,7 +6766,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>190</v>
       </c>
@@ -6681,7 +6807,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>69</v>
       </c>
@@ -6722,7 +6848,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -6763,7 +6889,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -6804,7 +6930,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -6845,7 +6971,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -6886,7 +7012,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>271</v>
       </c>
@@ -6927,7 +7053,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -6968,7 +7094,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>289</v>
       </c>
@@ -7009,7 +7135,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -7050,7 +7176,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>420</v>
       </c>
@@ -7091,7 +7217,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>110</v>
       </c>
@@ -7132,7 +7258,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>234</v>
       </c>
@@ -7173,7 +7299,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>88</v>
       </c>
@@ -7214,7 +7340,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -7255,7 +7381,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>249</v>
       </c>
@@ -7296,7 +7422,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>289</v>
       </c>
@@ -7337,7 +7463,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>190</v>
       </c>
@@ -7378,7 +7504,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>110</v>
       </c>
@@ -7419,7 +7545,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>318</v>
       </c>
@@ -7460,7 +7586,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>190</v>
       </c>
@@ -7501,7 +7627,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>420</v>
       </c>
@@ -7542,7 +7668,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>318</v>
       </c>
@@ -7583,7 +7709,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>446</v>
       </c>
@@ -7624,7 +7750,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>398</v>
       </c>
@@ -7665,7 +7791,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>361</v>
       </c>
@@ -7706,7 +7832,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>48</v>
       </c>
@@ -7747,7 +7873,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -7788,7 +7914,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>300</v>
       </c>
@@ -7829,7 +7955,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>190</v>
       </c>
@@ -7870,7 +7996,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>300</v>
       </c>
@@ -7911,7 +8037,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>154</v>
       </c>
@@ -7952,7 +8078,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>234</v>
       </c>
@@ -7993,7 +8119,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -8034,7 +8160,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>48</v>
       </c>
@@ -8075,7 +8201,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -8116,7 +8242,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>154</v>
       </c>
@@ -8157,7 +8283,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>175</v>
       </c>
@@ -8198,7 +8324,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>446</v>
       </c>
@@ -8239,7 +8365,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -8280,7 +8406,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>190</v>
       </c>
@@ -8321,7 +8447,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>420</v>
       </c>
@@ -8362,7 +8488,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -8403,7 +8529,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>289</v>
       </c>
@@ -8444,7 +8570,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>132</v>
       </c>
@@ -8485,7 +8611,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>446</v>
       </c>
@@ -8526,7 +8652,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>88</v>
       </c>
@@ -8567,7 +8693,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>26</v>
       </c>
@@ -8608,7 +8734,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>378</v>
       </c>
@@ -8649,7 +8775,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>339</v>
       </c>
@@ -8690,7 +8816,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>249</v>
       </c>
@@ -8731,7 +8857,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>110</v>
       </c>
@@ -8772,7 +8898,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>318</v>
       </c>
@@ -8813,7 +8939,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>420</v>
       </c>
@@ -8854,7 +8980,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>378</v>
       </c>
@@ -8895,7 +9021,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>110</v>
       </c>
@@ -8936,7 +9062,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>271</v>
       </c>
@@ -8977,7 +9103,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>110</v>
       </c>
@@ -9018,7 +9144,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>446</v>
       </c>
@@ -9059,7 +9185,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>234</v>
       </c>
@@ -9100,7 +9226,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>88</v>
       </c>
@@ -9141,7 +9267,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>398</v>
       </c>
@@ -9182,7 +9308,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>378</v>
       </c>
@@ -9223,7 +9349,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>361</v>
       </c>
@@ -9264,7 +9390,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>318</v>
       </c>
@@ -9305,7 +9431,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>110</v>
       </c>
@@ -9346,7 +9472,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>361</v>
       </c>
@@ -9387,7 +9513,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>249</v>
       </c>
@@ -9428,7 +9554,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -9469,7 +9595,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>300</v>
       </c>
@@ -9510,7 +9636,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>446</v>
       </c>
@@ -9551,7 +9677,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>339</v>
       </c>
@@ -9592,7 +9718,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>88</v>
       </c>
@@ -9633,7 +9759,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>212</v>
       </c>
@@ -9674,7 +9800,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>318</v>
       </c>
@@ -9712,7 +9838,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>420</v>
       </c>
@@ -9753,7 +9879,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>398</v>
       </c>
@@ -9794,7 +9920,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>132</v>
       </c>
@@ -9835,7 +9961,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>249</v>
       </c>
@@ -9876,7 +10002,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>175</v>
       </c>
@@ -9917,7 +10043,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>446</v>
       </c>
@@ -9958,7 +10084,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>378</v>
       </c>
@@ -9999,7 +10125,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>48</v>
       </c>
@@ -10040,7 +10166,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>154</v>
       </c>
@@ -10081,7 +10207,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>234</v>
       </c>
@@ -10122,7 +10248,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>249</v>
       </c>
@@ -10163,7 +10289,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>249</v>
       </c>
@@ -10204,7 +10330,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>234</v>
       </c>
@@ -10245,7 +10371,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>26</v>
       </c>
@@ -10286,7 +10412,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>378</v>
       </c>
@@ -10327,7 +10453,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>300</v>
       </c>
@@ -10368,7 +10494,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>339</v>
       </c>
@@ -10409,7 +10535,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>154</v>
       </c>
@@ -10450,7 +10576,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>378</v>
       </c>
@@ -10491,7 +10617,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>175</v>
       </c>
@@ -10532,7 +10658,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>420</v>
       </c>
@@ -10573,7 +10699,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>339</v>
       </c>
@@ -10614,7 +10740,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>249</v>
       </c>
@@ -10655,7 +10781,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>318</v>
       </c>
@@ -10696,7 +10822,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>212</v>
       </c>
@@ -10737,7 +10863,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>88</v>
       </c>
@@ -10778,7 +10904,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>271</v>
       </c>
@@ -10819,7 +10945,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>132</v>
       </c>
@@ -10860,7 +10986,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>234</v>
       </c>
@@ -10901,7 +11027,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>132</v>
       </c>
@@ -10942,7 +11068,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>212</v>
       </c>
@@ -10983,7 +11109,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>154</v>
       </c>
@@ -11024,7 +11150,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>234</v>
       </c>
@@ -11065,7 +11191,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>398</v>
       </c>
@@ -11106,7 +11232,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>212</v>
       </c>
@@ -11147,7 +11273,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>190</v>
       </c>
@@ -11188,7 +11314,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>300</v>
       </c>
@@ -11229,7 +11355,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>88</v>
       </c>
@@ -11270,7 +11396,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>132</v>
       </c>
@@ -11311,7 +11437,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>4</v>
       </c>
@@ -11352,7 +11478,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>300</v>
       </c>
@@ -11393,7 +11519,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>361</v>
       </c>
@@ -11434,7 +11560,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>132</v>
       </c>
@@ -11475,7 +11601,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>249</v>
       </c>
@@ -11516,7 +11642,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>26</v>
       </c>
@@ -11557,7 +11683,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>289</v>
       </c>
@@ -11598,7 +11724,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>4</v>
       </c>
@@ -11639,7 +11765,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -11680,7 +11806,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>398</v>
       </c>
@@ -11721,7 +11847,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>4</v>
       </c>
@@ -11762,7 +11888,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>190</v>
       </c>
@@ -11803,7 +11929,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>4</v>
       </c>
@@ -11844,7 +11970,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>318</v>
       </c>
@@ -11885,7 +12011,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>446</v>
       </c>
@@ -11926,7 +12052,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>271</v>
       </c>
@@ -11967,7 +12093,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>234</v>
       </c>
@@ -12008,7 +12134,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>212</v>
       </c>
@@ -12049,7 +12175,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>69</v>
       </c>
@@ -12090,7 +12216,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>339</v>
       </c>
@@ -12131,7 +12257,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>212</v>
       </c>
@@ -12172,7 +12298,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>132</v>
       </c>
@@ -12213,7 +12339,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>154</v>
       </c>
@@ -12254,7 +12380,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>4</v>
       </c>
@@ -12295,7 +12421,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="3" t="s">
         <v>435</v>
       </c>
@@ -12336,7 +12462,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>398</v>
       </c>
@@ -12377,7 +12503,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>378</v>
       </c>
@@ -12418,7 +12544,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>48</v>
       </c>
@@ -12459,7 +12585,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>249</v>
       </c>
@@ -12500,7 +12626,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>361</v>
       </c>
@@ -12541,7 +12667,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>154</v>
       </c>
@@ -12582,7 +12708,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>69</v>
       </c>
@@ -12623,7 +12749,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>175</v>
       </c>
@@ -12664,7 +12790,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>271</v>
       </c>
@@ -12705,7 +12831,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>271</v>
       </c>
@@ -12746,7 +12872,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>300</v>
       </c>
@@ -12787,7 +12913,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>132</v>
       </c>
@@ -12828,7 +12954,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>26</v>
       </c>
@@ -12869,7 +12995,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A203" s="4" t="s">
         <v>234</v>
       </c>
@@ -12910,7 +13036,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A204" s="4" t="s">
         <v>446</v>
       </c>
@@ -12951,7 +13077,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A205" s="4" t="s">
         <v>110</v>
       </c>
@@ -12992,7 +13118,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A206" s="4" t="s">
         <v>26</v>
       </c>
@@ -13033,7 +13159,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A207" s="4" t="s">
         <v>154</v>
       </c>
@@ -13074,7 +13200,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>234</v>
       </c>
@@ -13115,7 +13241,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>446</v>
       </c>
@@ -13156,7 +13282,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>26</v>
       </c>
@@ -13197,7 +13323,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>4</v>
       </c>
@@ -13238,7 +13364,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>300</v>
       </c>
@@ -13279,7 +13405,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>249</v>
       </c>
@@ -13320,7 +13446,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>378</v>
       </c>
@@ -13361,7 +13487,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>398</v>
       </c>
@@ -13402,7 +13528,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>361</v>
       </c>
@@ -13443,7 +13569,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>4</v>
       </c>
@@ -13484,7 +13610,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>420</v>
       </c>
@@ -13525,7 +13651,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>318</v>
       </c>
@@ -13566,7 +13692,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>339</v>
       </c>
@@ -13607,7 +13733,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>48</v>
       </c>
@@ -13648,7 +13774,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>339</v>
       </c>
@@ -13689,7 +13815,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>212</v>
       </c>
@@ -13730,7 +13856,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>88</v>
       </c>
@@ -13771,7 +13897,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>69</v>
       </c>
@@ -13812,7 +13938,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>26</v>
       </c>
@@ -13853,7 +13979,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>420</v>
       </c>
@@ -13894,7 +14020,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>190</v>
       </c>
@@ -13935,7 +14061,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>212</v>
       </c>
@@ -13976,7 +14102,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>26</v>
       </c>
@@ -14017,7 +14143,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>132</v>
       </c>
@@ -14055,7 +14181,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>88</v>
       </c>
@@ -14093,7 +14219,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>110</v>
       </c>
@@ -14134,7 +14260,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>212</v>
       </c>
@@ -14175,7 +14301,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>110</v>
       </c>
@@ -14216,7 +14342,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>4</v>
       </c>
@@ -14257,7 +14383,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>4</v>
       </c>
@@ -14298,7 +14424,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>378</v>
       </c>
@@ -14339,7 +14465,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>1290</v>
       </c>
@@ -14377,7 +14503,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>1290</v>
       </c>
@@ -14415,7 +14541,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>1290</v>
       </c>
@@ -14453,7 +14579,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>1290</v>
       </c>
@@ -14491,7 +14617,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>1290</v>
       </c>
@@ -14529,7 +14655,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>1290</v>
       </c>
@@ -14643,7 +14769,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>435</v>
       </c>
@@ -14684,7 +14810,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>1290</v>
       </c>
@@ -14725,7 +14851,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>1290</v>
       </c>
@@ -14766,7 +14892,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>1290</v>
       </c>
@@ -14807,8 +14933,436 @@
         <v>848</v>
       </c>
     </row>
+    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B251" s="2">
+        <v>31</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>1345</v>
+      </c>
+      <c r="D251" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E251" t="s">
+        <v>1354</v>
+      </c>
+      <c r="F251" t="s">
+        <v>1356</v>
+      </c>
+      <c r="G251" t="s">
+        <v>1355</v>
+      </c>
+      <c r="H251">
+        <v>2014</v>
+      </c>
+      <c r="I251" s="6">
+        <v>858914389</v>
+      </c>
+      <c r="J251" t="s">
+        <v>1357</v>
+      </c>
+      <c r="L251" s="2">
+        <v>1</v>
+      </c>
+      <c r="M251" s="6" t="s">
+        <v>1358</v>
+      </c>
+      <c r="N251">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="252" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B252" s="2">
+        <v>32</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D252" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E252" t="s">
+        <v>90</v>
+      </c>
+      <c r="F252" t="s">
+        <v>91</v>
+      </c>
+      <c r="G252" t="s">
+        <v>497</v>
+      </c>
+      <c r="H252">
+        <v>2019</v>
+      </c>
+      <c r="I252" t="s">
+        <v>821</v>
+      </c>
+      <c r="J252" t="s">
+        <v>822</v>
+      </c>
+      <c r="L252" s="2">
+        <v>1</v>
+      </c>
+      <c r="M252" t="s">
+        <v>1264</v>
+      </c>
+      <c r="N252">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="253" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B253" s="2">
+        <v>32</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D253" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E253" t="s">
+        <v>1359</v>
+      </c>
+      <c r="F253" t="s">
+        <v>1361</v>
+      </c>
+      <c r="G253" t="s">
+        <v>1360</v>
+      </c>
+      <c r="H253">
+        <v>2023</v>
+      </c>
+      <c r="I253">
+        <v>1379313397</v>
+      </c>
+      <c r="J253" t="s">
+        <v>1362</v>
+      </c>
+      <c r="L253" s="2">
+        <v>1</v>
+      </c>
+      <c r="M253" t="s">
+        <v>1363</v>
+      </c>
+      <c r="N253">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="254" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B254" s="2">
+        <v>32</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D254" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E254" t="s">
+        <v>1364</v>
+      </c>
+      <c r="F254" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G254" t="s">
+        <v>1366</v>
+      </c>
+      <c r="H254">
+        <v>1999</v>
+      </c>
+      <c r="I254">
+        <v>782888043</v>
+      </c>
+      <c r="J254" s="7" t="s">
+        <v>1368</v>
+      </c>
+      <c r="L254" s="2">
+        <v>1</v>
+      </c>
+      <c r="M254" t="s">
+        <v>1367</v>
+      </c>
+      <c r="N254">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="255" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B255" s="2">
+        <v>32</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D255" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E255" t="s">
+        <v>1369</v>
+      </c>
+      <c r="F255" t="s">
+        <v>1370</v>
+      </c>
+      <c r="G255" t="s">
+        <v>1371</v>
+      </c>
+      <c r="H255">
+        <v>2007</v>
+      </c>
+      <c r="I255">
+        <v>82672512</v>
+      </c>
+      <c r="J255" s="7" t="s">
+        <v>1373</v>
+      </c>
+      <c r="L255" s="2">
+        <v>1</v>
+      </c>
+      <c r="M255" t="s">
+        <v>1372</v>
+      </c>
+      <c r="N255">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="256" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B256" s="2">
+        <v>32</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D256" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E256" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F256" t="s">
+        <v>1375</v>
+      </c>
+      <c r="G256" t="s">
+        <v>1376</v>
+      </c>
+      <c r="H256">
+        <v>2020</v>
+      </c>
+      <c r="I256">
+        <v>1086015792</v>
+      </c>
+      <c r="J256" s="7" t="s">
+        <v>1378</v>
+      </c>
+      <c r="L256" s="2">
+        <v>1</v>
+      </c>
+      <c r="M256" t="s">
+        <v>1377</v>
+      </c>
+      <c r="N256">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="257" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B257" s="2">
+        <v>32</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D257" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E257" t="s">
+        <v>1379</v>
+      </c>
+      <c r="F257" t="s">
+        <v>1390</v>
+      </c>
+      <c r="G257" t="s">
+        <v>1388</v>
+      </c>
+      <c r="H257">
+        <v>2023</v>
+      </c>
+      <c r="I257" t="s">
+        <v>1391</v>
+      </c>
+      <c r="J257" s="7" t="s">
+        <v>1389</v>
+      </c>
+      <c r="L257" s="2">
+        <v>1</v>
+      </c>
+      <c r="M257" t="s">
+        <v>1392</v>
+      </c>
+      <c r="N257">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="258" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B258" s="2">
+        <v>32</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D258" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E258" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="259" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B259" s="2">
+        <v>32</v>
+      </c>
+      <c r="C259" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D259" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E259" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="260" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B260" s="2">
+        <v>32</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D260" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E260" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="261" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B261" s="2">
+        <v>32</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D261" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E261" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="262" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B262" s="2">
+        <v>32</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D262" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E262" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="263" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B263" s="2">
+        <v>32</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D263" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E263" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="264" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B264" s="2">
+        <v>32</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D264" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E264" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="265" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B265" s="2">
+        <v>32</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>1351</v>
+      </c>
+      <c r="D265" t="s">
+        <v>1316</v>
+      </c>
+      <c r="E265" t="s">
+        <v>1387</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:N250" xr:uid="{C17C54CB-A494-4D8A-8C6C-09250B011A75}">
+  <autoFilter ref="A1:N265" xr:uid="{C17C54CB-A494-4D8A-8C6C-09250B011A75}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Elif Ozcan"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N238">
       <sortCondition ref="M1:M238"/>
     </sortState>
@@ -14821,8 +15375,9 @@
     <hyperlink ref="G242" r:id="rId5" display="https://tudelft.on.worldcat.org/search?queryString=au%3D%22Essed%2C%20Philomena%22%20AND%20au%3D%221955%22&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{B51A4729-0139-4234-88FA-969F9304FE21}"/>
     <hyperlink ref="G244" r:id="rId6" display="https://tudelft.on.worldcat.org/search?queryString=au%3D%22Rand%2C%20Ayn%22&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{B7CFC170-C31E-46EB-A335-09BCADDA843B}"/>
     <hyperlink ref="E244" r:id="rId7" display="https://tudelft.on.worldcat.org/search/detail/71807799?queryString=the%20fountainhead&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{9928D475-0314-42CC-9268-6EEA844058FC}"/>
+    <hyperlink ref="G253" r:id="rId8" display="https://tudelft.on.worldcat.org/search?queryString=au%3D%22Elger%2C%20Dietmar%22&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{74CE4AEF-4228-4399-986C-37E9A5ADFD70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added all missing books (new recommenders)
</commit_message>
<xml_diff>
--- a/src/data/workshop_data/recommended_books.xlsx
+++ b/src/data/workshop_data/recommended_books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\workshop_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECF7F38-6D53-489E-A335-EF6B91C31F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E305CD-8618-4111-8B8F-88E542BBA383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{BE54A3D7-AD18-4D3A-9B07-972BEB6CC897}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2272" uniqueCount="1393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="1428">
   <si>
     <t>recommender</t>
   </si>
@@ -3622,12 +3622,6 @@
   </si>
   <si>
     <t>Michel Nadorp</t>
-  </si>
-  <si>
-    <t>51LKgvgK5HL._SY522_</t>
-  </si>
-  <si>
-    <t>51LKgvgK5HL._SY522_.webp</t>
   </si>
   <si>
     <t>This classic work, originally published in 1961, was written by Melvin Dresher, a RAND research mathematician, during the heyday of game theory research at RAND. The book introduces readers to the basic concepts of game theory and its applications for military, economic, and political problems, as well as its usefulness in decisionmaking in busines.</t>
@@ -4444,6 +4438,121 @@
   <si>
     <t>71Xo87sjRJL.webp</t>
   </si>
+  <si>
+    <t>Richard Yot</t>
+  </si>
+  <si>
+    <t>978-1786274519</t>
+  </si>
+  <si>
+    <t>1103977614.webp</t>
+  </si>
+  <si>
+    <t>This book is the first book to look at the way light can be used to create realistic and fantastical effects in a wide range of visual media. It is a valuable resource for animators, digital illustrators, painters, photographers, and artists working in any medium. Clearly written by a practicing illustrator, this book is essential reading for both students and professional artists.</t>
+  </si>
+  <si>
+    <t>978-1517900595</t>
+  </si>
+  <si>
+    <t>David Parisi</t>
+  </si>
+  <si>
+    <t>Since the rise of radio and television, we have lived in an era defined increasingly by the electronic circulation of images and sounds. But the flood of new computing technologies known as haptic interfaces—which use electricity, vibration, and force feedback to stimulate the sense of touch—offering an alternative way of mediating and experiencing reality. 
+In Archaeologies of Touch, David Parisi offers the first full history of these increasingly vital technologies, showing how the efforts of scientists and engineers over the past three hundred years have gradually remade and redefined our sense of touch. Through lively analyses of electrical machines, videogames, sex toys, sensory substitution systems, robotics, and human–computer interfaces, Parisi shows how the materiality of touch technologies has been shaped by attempts to transform humans into more efficient processors of information. 
+With haptics becoming ever more central to emerging virtual-reality platforms (immersive bodysuits loaded with touch-stimulating actuators), wearable computers (haptic messaging systems like the Apple Watch’s Taptic Engine), and smartphones (vibrations that emulate the feel of buttons and onscreen objects), Archaeologies of Touch offers a timely and provocative engagement with the long history of touch technology that helps us confront and question the power relations underpinning the project of giving touch its own set of technical media.</t>
+  </si>
+  <si>
+    <t>91B4C9183XL</t>
+  </si>
+  <si>
+    <t>91B4C9183XL.webp</t>
+  </si>
+  <si>
+    <t>1126217718.webp</t>
+  </si>
+  <si>
+    <t>The Touch is a new collaboration between Nathan Williams of Kinfolk and Jonas Bjerre-Poulsen of Norm Architects that welcome readers into over 25 inspiring spaces where interior design is not only visually appealing but engages all of the human senses. Through beautiful homes, hotels, museums, and retail stores--from contemporary designs by Ilse Crawford and Bijoy Jain to classic cases by Arne Jacobsen--readers are invited to explore how experiencing elements such as light, nature, materiality, color, and community can deliberately bring us back to our senses and imbue every day with a richer quality. In addition to stunning photography and interviews with design industry leaders as John Pawson and David Thulstrup, the book also details philosophical and art history references that reflect the tradition of design and color theory. For a deeper understanding of the concepts explored, The Touch includes an appendix which profiles architects such as Lina Bo Bardi and Richard Neutra. Heritage design pieces that helped influence this movement are also listed in the book.</t>
+  </si>
+  <si>
+    <t>John Clifford Burns</t>
+  </si>
+  <si>
+    <t>978-3899559781</t>
+  </si>
+  <si>
+    <t>Alva Noë</t>
+  </si>
+  <si>
+    <t>978-0809089161</t>
+  </si>
+  <si>
+    <t>962391614.webp</t>
+  </si>
+  <si>
+    <t>What is art? Why does it matter to us? What does it tell us about ourselves? Normally, we look to works of art in order to answer these fundamental questions. But what if the objects themselves are not what matter? in 'Strange Tools: Art and Human nature, ' the philosopher and cognitive scientist Alva Noë, art argues that our obsession with works of art has gotten in the way of understanding how art works on us. For Noë, art isn't a phenomenon in need of an explanation but a mode of research, a method of investigating what makes us human - a strange tool. Art isn't just something to look at or listen to - it is a challenge, a dare to try to make sense of what it is all about. Art aims not for satisfaction but for confrontation, intervention, and subversion. Through diverse and provocative examples from the history of art-making, Noë reveals the transformative power of artistic production. By staging a dance, choreographers cast light on the way bodily movement organizes us. Painting goes beyond depiction and representation to call into question the role of pictures in our lives. Accordingly, we cannot reduce art to some natural aesthetic sense or trigger; recent efforts to frame questions of art in terms of neurobiology and evolutionary theory alone are doomed to fail. By engaging with art, we are able to study ourselves in profoundly novel ways. In fact, art and philosophy have much more in common than you might think. Reframing the conversation around artists and their craft, 'Strange Tools' is a daring and stimulating intervention in contemporary thought.</t>
+  </si>
+  <si>
+    <t>978-0141035796</t>
+  </si>
+  <si>
+    <t>John Berger</t>
+  </si>
+  <si>
+    <t>Based on the BBC television series, John Berger's Ways of Seeing is a unique look at the way we view art, published as part of the Penguin on Design series in Penguin Modern Classics. 'Seeing comes before words. The child looks and recognizes before it can speak.'
+'But there is also another sense in which seeing comes before words. It is seeing which establishes our place in the surrounding world; we explain that world with words, but word can never undo the fact that we are surrounded by it. The relation between what we see and what we know is never settled.'
+John Berger's Ways of Seeing is one of the most stimulating and influential books on art in any language. First published in 1972, it was based on the BBC television series about which the Sunday Times critic commented: 'This is an eye-opener in more ways than one: by concentrating on how we look at paintings . . . he will almost certainly change the way you look at pictures.' By now he has.</t>
+  </si>
+  <si>
+    <t>97801410357.webp</t>
+  </si>
+  <si>
+    <t>978-0367271473</t>
+  </si>
+  <si>
+    <t>Andrew Knight-Hill</t>
+  </si>
+  <si>
+    <t>Sound and Image: Aesthetics and Practices brings together international artist scholars to explore diverse sound and image practices, applying critical perspectives to interrogate and evaluate both the aesthetics and practices that underpin the audiovisual. Contributions draw upon established discourses in electroacoustic music, media art history, film studies, critical theory and dance; framing and critiquing these arguments within the context of diverse audiovisual practices. The volume's interdisciplinary perspective contributes to the rich and evolving dialogue surrounding the audiovisual, demonstrating the value and significance of practice informed theory, and theory derived from practice. The ideas and approaches explored within this book will find application in a wide range of contexts across the whole scope of audiovisuality, from visual music and experimental film, to narrative film and documentary, to live performance, sound design and into sonic art and electroacoustic music. This book is ideal for artists, composers and researchers investigating theoretical positions and compositional practices which bring together sound and image.</t>
+  </si>
+  <si>
+    <t>1140369992.webp</t>
+  </si>
+  <si>
+    <t>First published in 1996, The Eyes of the Skin is a classic of architectural theory. It asks the far-reaching question why, when there are five senses, is one single sense -- sight -- so predominant in architectural culture and design? With the ascendancy of the digital and the all-pervasive use of the image electronically, the subject is all the more pressing and topical since the first edition's publication. Juhani Pallasmaa argues that the suppression of the other four sensory realms has led to the overall impoverishment of our built environment, often diminishing the emphasis on the spatial experience of a building and architecture's ability to inspire, engage and be wholly life enhancing. For a student reading this text for the first time, The Eyes of the Skin is a revelation. It provides a fresh, compelling insight into architectural culture which continues to inspire more than a quarter-century after its initial publication. This fourth edition presents the author's latest views on the emphasis of place, unfocused perception, sensory issues, and existential experience. It also includes updates and clarifications throughout, to reinforce how our sense of self in the world remains our most important sense and has the greatest impact on today's architecture.</t>
+  </si>
+  <si>
+    <t>Juhani Pallasmaa</t>
+  </si>
+  <si>
+    <t>978-1394200672</t>
+  </si>
+  <si>
+    <t>1412153743.webp</t>
+  </si>
+  <si>
+    <t>780815260.webp</t>
+  </si>
+  <si>
+    <t>Synesthetic design strives to develop products that systematically incorporate all five senses. In future, the current wealth of medical technical insights in psychology, physiology, motor functions, and neurology, and the development of innovative materials with astonishing new properties will open up almost unlimited opportunities for the designer's creativity. Haverkamp brings together, for the first time, precisely those aspects of this fundamental knowledge that are specifically relevant for designers. The result is a clear and well-organized handbook that offers designers of all schools a solid foundation for their own designs. Michael Haverkamp has been working on the concept of multi-sensory design for many years; he is an internationally recognized expert on sound design and synesthesia research in general.</t>
+  </si>
+  <si>
+    <t>Michael Haverkamp</t>
+  </si>
+  <si>
+    <t>978-3034607155</t>
+  </si>
+  <si>
+    <t>51LKgvgK5HL</t>
+  </si>
+  <si>
+    <t>51LKgvgK5HL.webp</t>
+  </si>
+  <si>
+    <t>1129098750.webp</t>
+  </si>
+  <si>
+    <t>839343829.webp</t>
+  </si>
 </sst>
 </file>
 
@@ -4522,7 +4631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4536,7 +4645,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4874,8 +4982,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E254" sqref="E254"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M255" sqref="M255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4901,7 +5009,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1157</v>
@@ -4945,7 +5053,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -4968,7 +5076,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -4991,7 +5099,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D4" t="s">
         <v>133</v>
@@ -5032,7 +5140,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -5073,7 +5181,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D6" t="s">
         <v>340</v>
@@ -5114,7 +5222,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -5155,7 +5263,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -5196,7 +5304,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -5237,7 +5345,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -5278,7 +5386,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D11" t="s">
         <v>191</v>
@@ -5319,7 +5427,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D12" t="s">
         <v>111</v>
@@ -5360,7 +5468,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -5383,7 +5491,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D14" t="s">
         <v>70</v>
@@ -5424,7 +5532,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D15" t="s">
         <v>340</v>
@@ -5465,7 +5573,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D16" t="s">
         <v>89</v>
@@ -5506,7 +5614,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -5529,7 +5637,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -5552,7 +5660,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D19" t="s">
         <v>191</v>
@@ -5564,22 +5672,22 @@
         <v>279</v>
       </c>
       <c r="G19" t="s">
-        <v>1196</v>
+        <v>1194</v>
       </c>
       <c r="H19">
         <v>2007</v>
       </c>
       <c r="I19" t="s">
+        <v>1424</v>
+      </c>
+      <c r="J19" t="s">
         <v>1193</v>
       </c>
-      <c r="J19" t="s">
-        <v>1195</v>
-      </c>
       <c r="L19" s="2">
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>1194</v>
+        <v>1425</v>
       </c>
       <c r="N19">
         <v>848</v>
@@ -5593,7 +5701,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D20" t="s">
         <v>340</v>
@@ -5605,22 +5713,22 @@
         <v>348</v>
       </c>
       <c r="G20" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="H20">
         <v>1998</v>
       </c>
       <c r="I20" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="J20" t="s">
+        <v>1235</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1</v>
+      </c>
+      <c r="M20" t="s">
         <v>1237</v>
-      </c>
-      <c r="L20" s="2">
-        <v>1</v>
-      </c>
-      <c r="M20" t="s">
-        <v>1239</v>
       </c>
       <c r="N20">
         <v>848</v>
@@ -5634,7 +5742,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D21" t="s">
         <v>250</v>
@@ -5646,22 +5754,22 @@
         <v>365</v>
       </c>
       <c r="G21" t="s">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="H21">
         <v>2004</v>
       </c>
       <c r="I21" t="s">
+        <v>1195</v>
+      </c>
+      <c r="J21" t="s">
         <v>1197</v>
       </c>
-      <c r="J21" t="s">
-        <v>1199</v>
-      </c>
       <c r="L21" s="2">
         <v>1</v>
       </c>
       <c r="M21" t="s">
-        <v>1198</v>
+        <v>1196</v>
       </c>
       <c r="N21">
         <v>848</v>
@@ -5675,7 +5783,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -5687,22 +5795,22 @@
         <v>166</v>
       </c>
       <c r="G22" t="s">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="H22">
         <v>1995</v>
       </c>
       <c r="I22" t="s">
+        <v>1199</v>
+      </c>
+      <c r="J22" t="s">
         <v>1201</v>
       </c>
-      <c r="J22" t="s">
-        <v>1203</v>
-      </c>
       <c r="L22" s="2">
         <v>1</v>
       </c>
       <c r="M22" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="N22">
         <v>848</v>
@@ -5716,7 +5824,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -5739,7 +5847,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
@@ -5751,22 +5859,22 @@
         <v>181</v>
       </c>
       <c r="G24" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="H24">
         <v>1996</v>
       </c>
       <c r="I24" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="J24" t="s">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="L24" s="2">
         <v>1</v>
       </c>
       <c r="M24" t="s">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="N24">
         <v>848</v>
@@ -5780,7 +5888,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D25" t="s">
         <v>191</v>
@@ -5792,22 +5900,22 @@
         <v>310</v>
       </c>
       <c r="G25" t="s">
-        <v>1211</v>
+        <v>1209</v>
       </c>
       <c r="H25">
         <v>1997</v>
       </c>
       <c r="I25" t="s">
+        <v>1208</v>
+      </c>
+      <c r="J25" t="s">
         <v>1210</v>
       </c>
-      <c r="J25" t="s">
-        <v>1212</v>
-      </c>
       <c r="L25" s="2">
         <v>1</v>
       </c>
       <c r="M25" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="N25">
         <v>848</v>
@@ -5821,7 +5929,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -5844,7 +5952,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D27" t="s">
         <v>191</v>
@@ -5853,25 +5961,25 @@
         <v>282</v>
       </c>
       <c r="F27" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="G27" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="H27">
         <v>1968</v>
       </c>
       <c r="I27" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="J27" t="s">
+        <v>1240</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
         <v>1242</v>
-      </c>
-      <c r="L27" s="2">
-        <v>1</v>
-      </c>
-      <c r="M27" t="s">
-        <v>1244</v>
       </c>
       <c r="N27">
         <v>848</v>
@@ -5885,7 +5993,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D28" t="s">
         <v>250</v>
@@ -5897,22 +6005,22 @@
         <v>375</v>
       </c>
       <c r="G28" t="s">
-        <v>1216</v>
+        <v>1214</v>
       </c>
       <c r="H28">
         <v>1999</v>
       </c>
       <c r="I28" t="s">
-        <v>1214</v>
+        <v>1212</v>
       </c>
       <c r="J28" t="s">
-        <v>1215</v>
+        <v>1213</v>
       </c>
       <c r="L28" s="2">
         <v>1</v>
       </c>
       <c r="M28" t="s">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="N28">
         <v>848</v>
@@ -5926,7 +6034,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -5949,7 +6057,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -5972,7 +6080,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D31" t="s">
         <v>70</v>
@@ -5981,25 +6089,25 @@
         <v>78</v>
       </c>
       <c r="F31" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="G31" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="H31">
         <v>2014</v>
       </c>
       <c r="I31" t="s">
+        <v>1244</v>
+      </c>
+      <c r="J31" t="s">
         <v>1246</v>
       </c>
-      <c r="J31" t="s">
-        <v>1248</v>
-      </c>
       <c r="L31" s="2">
         <v>1</v>
       </c>
       <c r="M31" t="s">
-        <v>1247</v>
+        <v>1245</v>
       </c>
       <c r="N31">
         <v>848</v>
@@ -6013,7 +6121,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D32" t="s">
         <v>70</v>
@@ -6025,22 +6133,22 @@
         <v>80</v>
       </c>
       <c r="G32" t="s">
-        <v>1217</v>
+        <v>1215</v>
       </c>
       <c r="H32">
         <v>2019</v>
       </c>
       <c r="I32" t="s">
-        <v>1220</v>
+        <v>1218</v>
       </c>
       <c r="J32" t="s">
-        <v>1218</v>
+        <v>1216</v>
       </c>
       <c r="L32" s="2">
         <v>1</v>
       </c>
       <c r="M32" t="s">
-        <v>1219</v>
+        <v>1217</v>
       </c>
       <c r="N32">
         <v>848</v>
@@ -6054,7 +6162,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -6066,22 +6174,22 @@
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="H33">
         <v>2007</v>
       </c>
       <c r="I33" t="s">
-        <v>1222</v>
+        <v>1220</v>
       </c>
       <c r="J33" t="s">
-        <v>1223</v>
+        <v>1221</v>
       </c>
       <c r="L33" s="2">
         <v>1</v>
       </c>
       <c r="M33" t="s">
-        <v>1221</v>
+        <v>1219</v>
       </c>
       <c r="N33">
         <v>848</v>
@@ -6095,7 +6203,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D34" t="s">
         <v>213</v>
@@ -6107,22 +6215,22 @@
         <v>223</v>
       </c>
       <c r="G34" t="s">
-        <v>1226</v>
+        <v>1224</v>
       </c>
       <c r="H34">
         <v>2000</v>
       </c>
       <c r="I34" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="J34" t="s">
-        <v>1225</v>
+        <v>1223</v>
       </c>
       <c r="L34" s="2">
         <v>1</v>
       </c>
       <c r="M34" t="s">
-        <v>1228</v>
+        <v>1226</v>
       </c>
       <c r="N34">
         <v>848</v>
@@ -6136,16 +6244,16 @@
         <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
       </c>
       <c r="E35" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="F35" t="s">
-        <v>1254</v>
+        <v>1252</v>
       </c>
       <c r="G35" t="s">
         <v>420</v>
@@ -6154,16 +6262,16 @@
         <v>2023</v>
       </c>
       <c r="I35" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="J35" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="L35" s="2">
         <v>1</v>
       </c>
       <c r="M35" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="N35">
         <v>848</v>
@@ -6177,7 +6285,7 @@
         <v>23</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D36" t="s">
         <v>191</v>
@@ -6189,22 +6297,22 @@
         <v>284</v>
       </c>
       <c r="G36" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
       <c r="H36">
         <v>1998</v>
       </c>
       <c r="I36" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="J36" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
       <c r="L36" s="2">
         <v>1</v>
       </c>
       <c r="M36" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="N36">
         <v>848</v>
@@ -6218,7 +6326,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D37" t="s">
         <v>70</v>
@@ -6227,25 +6335,25 @@
         <v>83</v>
       </c>
       <c r="F37" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="G37" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="H37">
         <v>2021</v>
       </c>
       <c r="I37" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="J37" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="L37" s="2">
         <v>1</v>
       </c>
       <c r="M37" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="N37">
         <v>848</v>
@@ -6259,7 +6367,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
@@ -6282,7 +6390,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D39" t="s">
         <v>340</v>
@@ -6294,22 +6402,22 @@
         <v>358</v>
       </c>
       <c r="G39" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="H39">
         <v>2009</v>
       </c>
       <c r="I39" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="J39" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
       <c r="L39" s="2">
         <v>1</v>
       </c>
       <c r="M39" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
       <c r="N39">
         <v>848</v>
@@ -6323,7 +6431,7 @@
         <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D40" t="s">
         <v>191</v>
@@ -6364,7 +6472,7 @@
         <v>18</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D41" t="s">
         <v>111</v>
@@ -6376,7 +6484,7 @@
         <v>117</v>
       </c>
       <c r="G41" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="H41">
         <v>2023</v>
@@ -6385,7 +6493,7 @@
         <v>805</v>
       </c>
       <c r="J41" t="s">
-        <v>1260</v>
+        <v>1258</v>
       </c>
       <c r="L41" s="2">
         <v>1</v>
@@ -6405,7 +6513,7 @@
         <v>24</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D42" t="s">
         <v>399</v>
@@ -6446,7 +6554,7 @@
         <v>14</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D43" t="s">
         <v>250</v>
@@ -6487,7 +6595,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D44" t="s">
         <v>191</v>
@@ -6528,7 +6636,7 @@
         <v>17</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D45" t="s">
         <v>133</v>
@@ -6569,7 +6677,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D46" t="s">
         <v>133</v>
@@ -6610,7 +6718,7 @@
         <v>24</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D47" t="s">
         <v>399</v>
@@ -6651,7 +6759,7 @@
         <v>6</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
@@ -6692,7 +6800,7 @@
         <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D49" t="s">
         <v>191</v>
@@ -6733,7 +6841,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D50" t="s">
         <v>399</v>
@@ -6774,7 +6882,7 @@
         <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D51" t="s">
         <v>191</v>
@@ -6815,7 +6923,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D52" t="s">
         <v>70</v>
@@ -6856,7 +6964,7 @@
         <v>21</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D53" t="s">
         <v>49</v>
@@ -6897,7 +7005,7 @@
         <v>21</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D54" t="s">
         <v>49</v>
@@ -6938,7 +7046,7 @@
         <v>5</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D55" t="s">
         <v>70</v>
@@ -6979,7 +7087,7 @@
         <v>30</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D56" t="s">
         <v>89</v>
@@ -7020,7 +7128,7 @@
         <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D57" t="s">
         <v>191</v>
@@ -7061,7 +7169,7 @@
         <v>21</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D58" t="s">
         <v>49</v>
@@ -7102,7 +7210,7 @@
         <v>27</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D59" t="s">
         <v>111</v>
@@ -7143,7 +7251,7 @@
         <v>21</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D60" t="s">
         <v>49</v>
@@ -7184,7 +7292,7 @@
         <v>6</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D61" t="s">
         <v>27</v>
@@ -7225,7 +7333,7 @@
         <v>18</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D62" t="s">
         <v>111</v>
@@ -7266,7 +7374,7 @@
         <v>19</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D63" t="s">
         <v>27</v>
@@ -7307,7 +7415,7 @@
         <v>30</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D64" t="s">
         <v>89</v>
@@ -7348,7 +7456,7 @@
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D65" t="s">
         <v>70</v>
@@ -7389,7 +7497,7 @@
         <v>4</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D66" t="s">
         <v>250</v>
@@ -7430,7 +7538,7 @@
         <v>27</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D67" t="s">
         <v>111</v>
@@ -7471,7 +7579,7 @@
         <v>22</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D68" t="s">
         <v>191</v>
@@ -7512,7 +7620,7 @@
         <v>18</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D69" t="s">
         <v>111</v>
@@ -7553,7 +7661,7 @@
         <v>17</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D70" t="s">
         <v>133</v>
@@ -7594,7 +7702,7 @@
         <v>22</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D71" t="s">
         <v>191</v>
@@ -7635,7 +7743,7 @@
         <v>6</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
@@ -7676,7 +7784,7 @@
         <v>17</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D73" t="s">
         <v>133</v>
@@ -7717,7 +7825,7 @@
         <v>8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D74" t="s">
         <v>27</v>
@@ -7758,7 +7866,7 @@
         <v>24</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D75" t="s">
         <v>399</v>
@@ -7799,7 +7907,7 @@
         <v>14</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D76" t="s">
         <v>250</v>
@@ -7820,7 +7928,7 @@
         <v>654</v>
       </c>
       <c r="J76" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="L76" s="2">
         <v>1</v>
@@ -7840,7 +7948,7 @@
         <v>21</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D77" t="s">
         <v>49</v>
@@ -7881,7 +7989,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D78" t="s">
         <v>27</v>
@@ -7922,7 +8030,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D79" t="s">
         <v>191</v>
@@ -7963,7 +8071,7 @@
         <v>22</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D80" t="s">
         <v>191</v>
@@ -8004,7 +8112,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D81" t="s">
         <v>191</v>
@@ -8025,7 +8133,7 @@
         <v>796</v>
       </c>
       <c r="J81" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="L81" s="2">
         <v>1</v>
@@ -8045,7 +8153,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
@@ -8086,7 +8194,7 @@
         <v>19</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
@@ -8127,7 +8235,7 @@
         <v>3</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D84" t="s">
         <v>27</v>
@@ -8168,7 +8276,7 @@
         <v>21</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D85" t="s">
         <v>49</v>
@@ -8209,7 +8317,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D86" t="s">
         <v>27</v>
@@ -8250,7 +8358,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D87" t="s">
         <v>27</v>
@@ -8291,7 +8399,7 @@
         <v>3</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D88" t="s">
         <v>27</v>
@@ -8332,7 +8440,7 @@
         <v>8</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D89" t="s">
         <v>27</v>
@@ -8373,7 +8481,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D90" t="s">
         <v>27</v>
@@ -8414,7 +8522,7 @@
         <v>22</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D91" t="s">
         <v>191</v>
@@ -8455,7 +8563,7 @@
         <v>6</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -8496,7 +8604,7 @@
         <v>3</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
@@ -8537,7 +8645,7 @@
         <v>27</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D94" t="s">
         <v>111</v>
@@ -8578,7 +8686,7 @@
         <v>7</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D95" t="s">
         <v>133</v>
@@ -8619,7 +8727,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D96" t="s">
         <v>27</v>
@@ -8660,7 +8768,7 @@
         <v>30</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D97" t="s">
         <v>89</v>
@@ -8701,7 +8809,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D98" t="s">
         <v>27</v>
@@ -8734,7 +8842,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>378</v>
       </c>
@@ -8742,7 +8850,7 @@
         <v>20</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D99" t="s">
         <v>340</v>
@@ -8783,7 +8891,7 @@
         <v>25</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D100" t="s">
         <v>340</v>
@@ -8824,7 +8932,7 @@
         <v>4</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D101" t="s">
         <v>250</v>
@@ -8865,7 +8973,7 @@
         <v>18</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D102" t="s">
         <v>111</v>
@@ -8906,7 +9014,7 @@
         <v>17</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D103" t="s">
         <v>133</v>
@@ -8947,7 +9055,7 @@
         <v>6</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D104" t="s">
         <v>27</v>
@@ -8988,7 +9096,7 @@
         <v>20</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D105" t="s">
         <v>340</v>
@@ -9029,7 +9137,7 @@
         <v>18</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D106" t="s">
         <v>111</v>
@@ -9070,7 +9178,7 @@
         <v>23</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D107" t="s">
         <v>191</v>
@@ -9111,7 +9219,7 @@
         <v>18</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D108" t="s">
         <v>111</v>
@@ -9152,7 +9260,7 @@
         <v>8</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D109" t="s">
         <v>27</v>
@@ -9193,7 +9301,7 @@
         <v>19</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -9214,7 +9322,7 @@
         <v>735</v>
       </c>
       <c r="J110" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="L110" s="2">
         <v>1</v>
@@ -9234,7 +9342,7 @@
         <v>30</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D111" t="s">
         <v>89</v>
@@ -9275,7 +9383,7 @@
         <v>24</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D112" t="s">
         <v>399</v>
@@ -9308,7 +9416,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>378</v>
       </c>
@@ -9316,7 +9424,7 @@
         <v>20</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D113" t="s">
         <v>340</v>
@@ -9357,7 +9465,7 @@
         <v>14</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D114" t="s">
         <v>250</v>
@@ -9398,7 +9506,7 @@
         <v>17</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D115" t="s">
         <v>133</v>
@@ -9439,7 +9547,7 @@
         <v>18</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D116" t="s">
         <v>111</v>
@@ -9480,7 +9588,7 @@
         <v>14</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D117" t="s">
         <v>250</v>
@@ -9521,7 +9629,7 @@
         <v>4</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D118" t="s">
         <v>250</v>
@@ -9562,7 +9670,7 @@
         <v>14</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D119" t="s">
         <v>250</v>
@@ -9603,7 +9711,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D120" t="s">
         <v>191</v>
@@ -9644,7 +9752,7 @@
         <v>8</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D121" t="s">
         <v>27</v>
@@ -9665,7 +9773,7 @@
         <v>688</v>
       </c>
       <c r="J121" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="L121" s="2">
         <v>1</v>
@@ -9685,7 +9793,7 @@
         <v>25</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D122" t="s">
         <v>340</v>
@@ -9726,7 +9834,7 @@
         <v>30</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D123" t="s">
         <v>89</v>
@@ -9767,7 +9875,7 @@
         <v>26</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D124" t="s">
         <v>213</v>
@@ -9808,7 +9916,7 @@
         <v>17</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D125" t="s">
         <v>133</v>
@@ -9846,7 +9954,7 @@
         <v>6</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D126" t="s">
         <v>27</v>
@@ -9887,7 +9995,7 @@
         <v>24</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D127" t="s">
         <v>399</v>
@@ -9928,7 +10036,7 @@
         <v>7</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D128" t="s">
         <v>133</v>
@@ -9969,7 +10077,7 @@
         <v>4</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D129" t="s">
         <v>250</v>
@@ -10010,7 +10118,7 @@
         <v>3</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D130" t="s">
         <v>27</v>
@@ -10051,7 +10159,7 @@
         <v>8</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D131" t="s">
         <v>27</v>
@@ -10092,7 +10200,7 @@
         <v>20</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D132" t="s">
         <v>340</v>
@@ -10133,7 +10241,7 @@
         <v>21</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D133" t="s">
         <v>49</v>
@@ -10174,7 +10282,7 @@
         <v>2</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D134" t="s">
         <v>27</v>
@@ -10215,7 +10323,7 @@
         <v>19</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D135" t="s">
         <v>27</v>
@@ -10256,7 +10364,7 @@
         <v>4</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D136" t="s">
         <v>250</v>
@@ -10297,7 +10405,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D137" t="s">
         <v>250</v>
@@ -10338,7 +10446,7 @@
         <v>19</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D138" t="s">
         <v>27</v>
@@ -10379,7 +10487,7 @@
         <v>13</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D139" t="s">
         <v>27</v>
@@ -10420,7 +10528,7 @@
         <v>20</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D140" t="s">
         <v>340</v>
@@ -10461,7 +10569,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D141" t="s">
         <v>191</v>
@@ -10502,7 +10610,7 @@
         <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D142" t="s">
         <v>340</v>
@@ -10543,7 +10651,7 @@
         <v>2</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D143" t="s">
         <v>27</v>
@@ -10584,7 +10692,7 @@
         <v>20</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D144" t="s">
         <v>340</v>
@@ -10625,7 +10733,7 @@
         <v>3</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D145" t="s">
         <v>27</v>
@@ -10666,7 +10774,7 @@
         <v>6</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D146" t="s">
         <v>27</v>
@@ -10699,7 +10807,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>339</v>
       </c>
@@ -10707,7 +10815,7 @@
         <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D147" t="s">
         <v>340</v>
@@ -10748,7 +10856,7 @@
         <v>4</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D148" t="s">
         <v>250</v>
@@ -10789,7 +10897,7 @@
         <v>17</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D149" t="s">
         <v>133</v>
@@ -10830,7 +10938,7 @@
         <v>26</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D150" t="s">
         <v>213</v>
@@ -10871,7 +10979,7 @@
         <v>30</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D151" t="s">
         <v>89</v>
@@ -10912,7 +11020,7 @@
         <v>23</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D152" t="s">
         <v>191</v>
@@ -10953,7 +11061,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D153" t="s">
         <v>133</v>
@@ -10994,7 +11102,7 @@
         <v>19</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D154" t="s">
         <v>27</v>
@@ -11035,7 +11143,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D155" t="s">
         <v>133</v>
@@ -11076,7 +11184,7 @@
         <v>26</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D156" t="s">
         <v>213</v>
@@ -11117,7 +11225,7 @@
         <v>2</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D157" t="s">
         <v>27</v>
@@ -11158,7 +11266,7 @@
         <v>19</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D158" t="s">
         <v>27</v>
@@ -11199,7 +11307,7 @@
         <v>24</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D159" t="s">
         <v>399</v>
@@ -11240,7 +11348,7 @@
         <v>26</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D160" t="s">
         <v>213</v>
@@ -11281,7 +11389,7 @@
         <v>22</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D161" t="s">
         <v>191</v>
@@ -11322,7 +11430,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D162" t="s">
         <v>191</v>
@@ -11363,7 +11471,7 @@
         <v>30</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D163" t="s">
         <v>89</v>
@@ -11404,7 +11512,7 @@
         <v>7</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D164" t="s">
         <v>133</v>
@@ -11445,7 +11553,7 @@
         <v>28</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D165" t="s">
         <v>5</v>
@@ -11486,7 +11594,7 @@
         <v>1</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D166" t="s">
         <v>191</v>
@@ -11527,7 +11635,7 @@
         <v>14</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D167" t="s">
         <v>250</v>
@@ -11568,7 +11676,7 @@
         <v>7</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D168" t="s">
         <v>133</v>
@@ -11609,7 +11717,7 @@
         <v>4</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D169" t="s">
         <v>250</v>
@@ -11650,7 +11758,7 @@
         <v>13</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D170" t="s">
         <v>27</v>
@@ -11691,7 +11799,7 @@
         <v>27</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D171" t="s">
         <v>111</v>
@@ -11732,7 +11840,7 @@
         <v>28</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D172" t="s">
         <v>5</v>
@@ -11773,7 +11881,7 @@
         <v>21</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D173" t="s">
         <v>49</v>
@@ -11814,7 +11922,7 @@
         <v>24</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D174" t="s">
         <v>399</v>
@@ -11855,7 +11963,7 @@
         <v>28</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D175" t="s">
         <v>5</v>
@@ -11896,7 +12004,7 @@
         <v>22</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D176" t="s">
         <v>191</v>
@@ -11937,7 +12045,7 @@
         <v>28</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D177" t="s">
         <v>5</v>
@@ -11978,7 +12086,7 @@
         <v>17</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D178" t="s">
         <v>133</v>
@@ -12019,7 +12127,7 @@
         <v>8</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D179" t="s">
         <v>27</v>
@@ -12040,7 +12148,7 @@
         <v>771</v>
       </c>
       <c r="J179" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="L179" s="2">
         <v>1</v>
@@ -12060,7 +12168,7 @@
         <v>23</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D180" t="s">
         <v>191</v>
@@ -12101,7 +12209,7 @@
         <v>19</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D181" t="s">
         <v>27</v>
@@ -12142,7 +12250,7 @@
         <v>26</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D182" t="s">
         <v>213</v>
@@ -12183,7 +12291,7 @@
         <v>5</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D183" t="s">
         <v>70</v>
@@ -12224,7 +12332,7 @@
         <v>25</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D184" t="s">
         <v>340</v>
@@ -12265,7 +12373,7 @@
         <v>26</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D185" t="s">
         <v>213</v>
@@ -12306,7 +12414,7 @@
         <v>7</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D186" t="s">
         <v>133</v>
@@ -12347,7 +12455,7 @@
         <v>2</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D187" t="s">
         <v>27</v>
@@ -12388,7 +12496,7 @@
         <v>28</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D188" t="s">
         <v>5</v>
@@ -12429,7 +12537,7 @@
         <v>29</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D189" t="s">
         <v>5</v>
@@ -12470,7 +12578,7 @@
         <v>24</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D190" t="s">
         <v>399</v>
@@ -12511,7 +12619,7 @@
         <v>20</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D191" t="s">
         <v>340</v>
@@ -12552,7 +12660,7 @@
         <v>21</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D192" t="s">
         <v>49</v>
@@ -12593,7 +12701,7 @@
         <v>4</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D193" t="s">
         <v>250</v>
@@ -12634,7 +12742,7 @@
         <v>14</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D194" t="s">
         <v>250</v>
@@ -12675,7 +12783,7 @@
         <v>2</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D195" t="s">
         <v>27</v>
@@ -12716,7 +12824,7 @@
         <v>5</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D196" t="s">
         <v>70</v>
@@ -12757,7 +12865,7 @@
         <v>3</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D197" t="s">
         <v>27</v>
@@ -12798,7 +12906,7 @@
         <v>23</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D198" t="s">
         <v>191</v>
@@ -12839,7 +12947,7 @@
         <v>23</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D199" t="s">
         <v>191</v>
@@ -12880,7 +12988,7 @@
         <v>1</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D200" t="s">
         <v>191</v>
@@ -12921,7 +13029,7 @@
         <v>7</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D201" t="s">
         <v>133</v>
@@ -12962,7 +13070,7 @@
         <v>13</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D202" t="s">
         <v>27</v>
@@ -13003,7 +13111,7 @@
         <v>19</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D203" t="s">
         <v>27</v>
@@ -13044,7 +13152,7 @@
         <v>8</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D204" t="s">
         <v>27</v>
@@ -13085,7 +13193,7 @@
         <v>18</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D205" t="s">
         <v>111</v>
@@ -13126,7 +13234,7 @@
         <v>13</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D206" t="s">
         <v>27</v>
@@ -13167,7 +13275,7 @@
         <v>2</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D207" t="s">
         <v>27</v>
@@ -13208,7 +13316,7 @@
         <v>19</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>1353</v>
+        <v>1351</v>
       </c>
       <c r="D208" t="s">
         <v>27</v>
@@ -13249,7 +13357,7 @@
         <v>8</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D209" t="s">
         <v>27</v>
@@ -13290,7 +13398,7 @@
         <v>13</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D210" t="s">
         <v>27</v>
@@ -13331,7 +13439,7 @@
         <v>28</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D211" t="s">
         <v>5</v>
@@ -13372,7 +13480,7 @@
         <v>1</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D212" t="s">
         <v>191</v>
@@ -13413,7 +13521,7 @@
         <v>4</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D213" t="s">
         <v>250</v>
@@ -13454,7 +13562,7 @@
         <v>20</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D214" t="s">
         <v>340</v>
@@ -13495,7 +13603,7 @@
         <v>24</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D215" t="s">
         <v>399</v>
@@ -13536,7 +13644,7 @@
         <v>14</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D216" t="s">
         <v>250</v>
@@ -13577,7 +13685,7 @@
         <v>28</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D217" t="s">
         <v>5</v>
@@ -13618,7 +13726,7 @@
         <v>6</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D218" t="s">
         <v>27</v>
@@ -13659,7 +13767,7 @@
         <v>17</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D219" t="s">
         <v>133</v>
@@ -13700,7 +13808,7 @@
         <v>25</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D220" t="s">
         <v>340</v>
@@ -13741,7 +13849,7 @@
         <v>21</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>1352</v>
+        <v>1350</v>
       </c>
       <c r="D221" t="s">
         <v>49</v>
@@ -13768,7 +13876,7 @@
         <v>1</v>
       </c>
       <c r="M221" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="N221">
         <v>848</v>
@@ -13782,7 +13890,7 @@
         <v>25</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D222" t="s">
         <v>340</v>
@@ -13809,7 +13917,7 @@
         <v>1</v>
       </c>
       <c r="M222" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="N222">
         <v>848</v>
@@ -13823,7 +13931,7 @@
         <v>26</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D223" t="s">
         <v>213</v>
@@ -13850,7 +13958,7 @@
         <v>1</v>
       </c>
       <c r="M223" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="N223">
         <v>848</v>
@@ -13864,7 +13972,7 @@
         <v>30</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D224" t="s">
         <v>89</v>
@@ -13891,7 +13999,7 @@
         <v>1</v>
       </c>
       <c r="M224" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="N224">
         <v>848</v>
@@ -13905,7 +14013,7 @@
         <v>5</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D225" t="s">
         <v>70</v>
@@ -13932,7 +14040,7 @@
         <v>1</v>
       </c>
       <c r="M225" t="s">
-        <v>1265</v>
+        <v>1263</v>
       </c>
       <c r="N225">
         <v>848</v>
@@ -13946,7 +14054,7 @@
         <v>13</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D226" t="s">
         <v>27</v>
@@ -13973,7 +14081,7 @@
         <v>1</v>
       </c>
       <c r="M226" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="N226">
         <v>848</v>
@@ -13987,7 +14095,7 @@
         <v>6</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D227" t="s">
         <v>27</v>
@@ -14014,7 +14122,7 @@
         <v>1</v>
       </c>
       <c r="M227" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="N227">
         <v>848</v>
@@ -14028,7 +14136,7 @@
         <v>22</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D228" t="s">
         <v>191</v>
@@ -14055,7 +14163,7 @@
         <v>1</v>
       </c>
       <c r="M228" t="s">
-        <v>1267</v>
+        <v>1265</v>
       </c>
       <c r="N228">
         <v>848</v>
@@ -14069,7 +14177,7 @@
         <v>26</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D229" t="s">
         <v>213</v>
@@ -14096,7 +14204,7 @@
         <v>1</v>
       </c>
       <c r="M229" t="s">
-        <v>1268</v>
+        <v>1266</v>
       </c>
       <c r="N229">
         <v>848</v>
@@ -14110,7 +14218,7 @@
         <v>13</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D230" t="s">
         <v>27</v>
@@ -14137,7 +14245,7 @@
         <v>1</v>
       </c>
       <c r="M230" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="N230">
         <v>848</v>
@@ -14151,7 +14259,7 @@
         <v>7</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D231" t="s">
         <v>133</v>
@@ -14175,7 +14283,7 @@
         <v>1</v>
       </c>
       <c r="M231" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="N231">
         <v>848</v>
@@ -14189,7 +14297,7 @@
         <v>30</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D232" t="s">
         <v>89</v>
@@ -14213,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="M232" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="N232">
         <v>848</v>
@@ -14227,7 +14335,7 @@
         <v>18</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D233" t="s">
         <v>111</v>
@@ -14239,7 +14347,7 @@
         <v>119</v>
       </c>
       <c r="G233" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="H233">
         <v>2012</v>
@@ -14248,13 +14356,13 @@
         <v>681</v>
       </c>
       <c r="J233" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="L233" s="2">
         <v>1</v>
       </c>
       <c r="M233" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="N233">
         <v>848</v>
@@ -14268,7 +14376,7 @@
         <v>26</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D234" t="s">
         <v>213</v>
@@ -14289,13 +14397,13 @@
         <v>698</v>
       </c>
       <c r="J234" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="L234" s="2">
         <v>1</v>
       </c>
       <c r="M234" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="N234">
         <v>848</v>
@@ -14309,7 +14417,7 @@
         <v>18</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D235" t="s">
         <v>111</v>
@@ -14330,13 +14438,13 @@
         <v>699</v>
       </c>
       <c r="J235" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="L235" s="2">
         <v>1</v>
       </c>
       <c r="M235" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="N235">
         <v>848</v>
@@ -14350,7 +14458,7 @@
         <v>28</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D236" t="s">
         <v>5</v>
@@ -14371,13 +14479,13 @@
         <v>727</v>
       </c>
       <c r="J236" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="L236" s="2">
         <v>1</v>
       </c>
       <c r="M236" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="N236">
         <v>848</v>
@@ -14391,7 +14499,7 @@
         <v>28</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D237" t="s">
         <v>5</v>
@@ -14412,13 +14520,13 @@
         <v>784</v>
       </c>
       <c r="J237" s="5" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="L237" s="2">
         <v>1</v>
       </c>
       <c r="M237" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="N237">
         <v>848</v>
@@ -14432,7 +14540,7 @@
         <v>20</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D238" t="s">
         <v>340</v>
@@ -14453,13 +14561,13 @@
         <v>785</v>
       </c>
       <c r="J238" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="L238" s="2">
         <v>1</v>
       </c>
       <c r="M238" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="N238">
         <v>848</v>
@@ -14467,25 +14575,25 @@
     </row>
     <row r="239" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B239" s="2">
         <v>31</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D239" t="s">
+        <v>1288</v>
+      </c>
+      <c r="E239" t="s">
+        <v>1289</v>
+      </c>
+      <c r="F239" t="s">
+        <v>1291</v>
+      </c>
+      <c r="G239" t="s">
         <v>1290</v>
-      </c>
-      <c r="E239" t="s">
-        <v>1291</v>
-      </c>
-      <c r="F239" t="s">
-        <v>1293</v>
-      </c>
-      <c r="G239" t="s">
-        <v>1292</v>
       </c>
       <c r="H239">
         <v>2023</v>
@@ -14494,7 +14602,7 @@
         <v>1362866564</v>
       </c>
       <c r="J239" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="L239" s="2">
         <v>1</v>
@@ -14505,25 +14613,25 @@
     </row>
     <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B240" s="2">
         <v>31</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D240" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E240" t="s">
+        <v>1293</v>
+      </c>
+      <c r="F240" t="s">
+        <v>1296</v>
+      </c>
+      <c r="G240" t="s">
         <v>1295</v>
-      </c>
-      <c r="F240" t="s">
-        <v>1298</v>
-      </c>
-      <c r="G240" t="s">
-        <v>1297</v>
       </c>
       <c r="H240">
         <v>2024</v>
@@ -14532,7 +14640,7 @@
         <v>1378931447</v>
       </c>
       <c r="J240" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="L240" s="2">
         <v>1</v>
@@ -14543,25 +14651,25 @@
     </row>
     <row r="241" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B241" s="2">
         <v>31</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D241" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E241" t="s">
+        <v>1297</v>
+      </c>
+      <c r="F241" t="s">
         <v>1299</v>
       </c>
-      <c r="F241" t="s">
-        <v>1301</v>
-      </c>
       <c r="G241" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="H241">
         <v>2021</v>
@@ -14570,7 +14678,7 @@
         <v>1354951065</v>
       </c>
       <c r="J241" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="L241" s="2">
         <v>1</v>
@@ -14581,25 +14689,25 @@
     </row>
     <row r="242" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B242" s="2">
         <v>31</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D242" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E242" t="s">
+        <v>1301</v>
+      </c>
+      <c r="F242" t="s">
+        <v>1302</v>
+      </c>
+      <c r="G242" t="s">
         <v>1303</v>
-      </c>
-      <c r="F242" t="s">
-        <v>1304</v>
-      </c>
-      <c r="G242" t="s">
-        <v>1305</v>
       </c>
       <c r="H242">
         <v>1991</v>
@@ -14608,7 +14716,7 @@
         <v>23972182</v>
       </c>
       <c r="J242" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="L242" s="2">
         <v>1</v>
@@ -14619,25 +14727,25 @@
     </row>
     <row r="243" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B243" s="2">
         <v>31</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D243" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E243" t="s">
+        <v>1305</v>
+      </c>
+      <c r="F243" t="s">
+        <v>1306</v>
+      </c>
+      <c r="G243" t="s">
         <v>1307</v>
-      </c>
-      <c r="F243" t="s">
-        <v>1308</v>
-      </c>
-      <c r="G243" t="s">
-        <v>1309</v>
       </c>
       <c r="H243">
         <v>2023</v>
@@ -14646,7 +14754,7 @@
         <v>1369522939</v>
       </c>
       <c r="J243" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="L243" s="2">
         <v>1</v>
@@ -14657,25 +14765,25 @@
     </row>
     <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B244" s="2">
         <v>31</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D244" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E244" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="F244" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="G244" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="H244">
         <v>2007</v>
@@ -14684,7 +14792,7 @@
         <v>71807799</v>
       </c>
       <c r="J244" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="L244" s="2">
         <v>1</v>
@@ -14693,27 +14801,27 @@
         <v>848</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B245" s="2">
         <v>32</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D245" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E245" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="F245" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="G245" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="H245">
         <v>2020</v>
@@ -14722,10 +14830,13 @@
         <v>1129098750</v>
       </c>
       <c r="J245" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="L245" s="2">
         <v>1</v>
+      </c>
+      <c r="M245" t="s">
+        <v>1426</v>
       </c>
       <c r="N245">
         <v>848</v>
@@ -14733,25 +14844,25 @@
     </row>
     <row r="246" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B246" s="2">
         <v>32</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D246" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E246" t="s">
+        <v>1317</v>
+      </c>
+      <c r="F246" t="s">
         <v>1319</v>
       </c>
-      <c r="F246" t="s">
-        <v>1321</v>
-      </c>
       <c r="G246" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="H246">
         <v>2005</v>
@@ -14760,10 +14871,13 @@
         <v>839343829</v>
       </c>
       <c r="J246" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="L246" s="2">
         <v>1</v>
+      </c>
+      <c r="M246" t="s">
+        <v>1427</v>
       </c>
       <c r="N246">
         <v>848</v>
@@ -14777,19 +14891,19 @@
         <v>29</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D247" t="s">
         <v>5</v>
       </c>
       <c r="E247" t="s">
+        <v>1322</v>
+      </c>
+      <c r="F247" t="s">
+        <v>1323</v>
+      </c>
+      <c r="G247" t="s">
         <v>1324</v>
-      </c>
-      <c r="F247" t="s">
-        <v>1325</v>
-      </c>
-      <c r="G247" t="s">
-        <v>1326</v>
       </c>
       <c r="H247">
         <v>2020</v>
@@ -14798,13 +14912,13 @@
         <v>1327959423</v>
       </c>
       <c r="J247" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="L247" s="2">
         <v>1</v>
       </c>
       <c r="M247" s="3" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="N247">
         <v>848</v>
@@ -14812,25 +14926,25 @@
     </row>
     <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B248" s="2">
         <v>31</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D248" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E248" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
       <c r="F248" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="G248" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="H248">
         <v>2016</v>
@@ -14839,13 +14953,13 @@
         <v>950569633</v>
       </c>
       <c r="J248" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
       <c r="L248" s="2">
         <v>1</v>
       </c>
       <c r="M248" s="3" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="N248">
         <v>848</v>
@@ -14853,25 +14967,25 @@
     </row>
     <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B249" s="2">
         <v>31</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D249" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E249" t="s">
+        <v>1330</v>
+      </c>
+      <c r="F249" t="s">
+        <v>1331</v>
+      </c>
+      <c r="G249" t="s">
         <v>1332</v>
-      </c>
-      <c r="F249" t="s">
-        <v>1333</v>
-      </c>
-      <c r="G249" t="s">
-        <v>1334</v>
       </c>
       <c r="H249">
         <v>2022</v>
@@ -14880,13 +14994,13 @@
         <v>1286804805</v>
       </c>
       <c r="J249" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="L249" s="2">
         <v>1</v>
       </c>
       <c r="M249" s="3" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="N249">
         <v>848</v>
@@ -14894,25 +15008,25 @@
     </row>
     <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B250" s="2">
         <v>31</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D250" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E250" t="s">
+        <v>1334</v>
+      </c>
+      <c r="F250" t="s">
+        <v>1335</v>
+      </c>
+      <c r="G250" t="s">
         <v>1336</v>
-      </c>
-      <c r="F250" t="s">
-        <v>1337</v>
-      </c>
-      <c r="G250" t="s">
-        <v>1338</v>
       </c>
       <c r="H250">
         <v>2023</v>
@@ -14921,13 +15035,13 @@
         <v>1452966194</v>
       </c>
       <c r="J250" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="L250" s="2">
         <v>1</v>
       </c>
       <c r="M250" s="3" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="N250">
         <v>848</v>
@@ -14935,25 +15049,25 @@
     </row>
     <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="B251" s="2">
         <v>31</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D251" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="E251" t="s">
+        <v>1352</v>
+      </c>
+      <c r="F251" t="s">
         <v>1354</v>
       </c>
-      <c r="F251" t="s">
-        <v>1356</v>
-      </c>
       <c r="G251" t="s">
-        <v>1355</v>
+        <v>1353</v>
       </c>
       <c r="H251">
         <v>2014</v>
@@ -14962,30 +15076,30 @@
         <v>858914389</v>
       </c>
       <c r="J251" t="s">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="L251" s="2">
         <v>1</v>
       </c>
       <c r="M251" s="6" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="N251">
         <v>848</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B252" s="2">
         <v>32</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D252" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E252" t="s">
         <v>90</v>
@@ -15009,33 +15123,33 @@
         <v>1</v>
       </c>
       <c r="M252" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="N252">
         <v>848</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B253" s="2">
         <v>32</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D253" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E253" t="s">
+        <v>1357</v>
+      </c>
+      <c r="F253" t="s">
         <v>1359</v>
       </c>
-      <c r="F253" t="s">
-        <v>1361</v>
-      </c>
       <c r="G253" t="s">
-        <v>1360</v>
+        <v>1358</v>
       </c>
       <c r="H253">
         <v>2023</v>
@@ -15044,39 +15158,39 @@
         <v>1379313397</v>
       </c>
       <c r="J253" t="s">
-        <v>1362</v>
+        <v>1360</v>
       </c>
       <c r="L253" s="2">
         <v>1</v>
       </c>
       <c r="M253" t="s">
-        <v>1363</v>
+        <v>1361</v>
       </c>
       <c r="N253">
         <v>848</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B254" s="2">
         <v>32</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D254" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E254" t="s">
+        <v>1362</v>
+      </c>
+      <c r="F254" t="s">
+        <v>1363</v>
+      </c>
+      <c r="G254" t="s">
         <v>1364</v>
-      </c>
-      <c r="F254" t="s">
-        <v>1365</v>
-      </c>
-      <c r="G254" t="s">
-        <v>1366</v>
       </c>
       <c r="H254">
         <v>1999</v>
@@ -15084,14 +15198,14 @@
       <c r="I254">
         <v>782888043</v>
       </c>
-      <c r="J254" s="7" t="s">
-        <v>1368</v>
+      <c r="J254" t="s">
+        <v>1366</v>
       </c>
       <c r="L254" s="2">
         <v>1</v>
       </c>
       <c r="M254" t="s">
-        <v>1367</v>
+        <v>1365</v>
       </c>
       <c r="N254">
         <v>848</v>
@@ -15099,25 +15213,25 @@
     </row>
     <row r="255" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B255" s="2">
         <v>32</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D255" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E255" t="s">
+        <v>1367</v>
+      </c>
+      <c r="F255" t="s">
+        <v>1368</v>
+      </c>
+      <c r="G255" t="s">
         <v>1369</v>
-      </c>
-      <c r="F255" t="s">
-        <v>1370</v>
-      </c>
-      <c r="G255" t="s">
-        <v>1371</v>
       </c>
       <c r="H255">
         <v>2007</v>
@@ -15125,40 +15239,40 @@
       <c r="I255">
         <v>82672512</v>
       </c>
-      <c r="J255" s="7" t="s">
-        <v>1373</v>
+      <c r="J255" t="s">
+        <v>1371</v>
       </c>
       <c r="L255" s="2">
         <v>1</v>
       </c>
       <c r="M255" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="N255">
         <v>848</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B256" s="2">
         <v>32</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D256" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E256" t="s">
+        <v>1372</v>
+      </c>
+      <c r="F256" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G256" t="s">
         <v>1374</v>
-      </c>
-      <c r="F256" t="s">
-        <v>1375</v>
-      </c>
-      <c r="G256" t="s">
-        <v>1376</v>
       </c>
       <c r="H256">
         <v>2020</v>
@@ -15166,201 +15280,397 @@
       <c r="I256">
         <v>1086015792</v>
       </c>
-      <c r="J256" s="7" t="s">
-        <v>1378</v>
+      <c r="J256" t="s">
+        <v>1376</v>
       </c>
       <c r="L256" s="2">
         <v>1</v>
       </c>
       <c r="M256" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="N256">
         <v>848</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B257" s="2">
         <v>32</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D257" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E257" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="F257" t="s">
-        <v>1390</v>
+        <v>1388</v>
       </c>
       <c r="G257" t="s">
-        <v>1388</v>
+        <v>1386</v>
       </c>
       <c r="H257">
         <v>2023</v>
       </c>
       <c r="I257" t="s">
-        <v>1391</v>
-      </c>
-      <c r="J257" s="7" t="s">
         <v>1389</v>
       </c>
+      <c r="J257" t="s">
+        <v>1387</v>
+      </c>
       <c r="L257" s="2">
         <v>1</v>
       </c>
       <c r="M257" t="s">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="N257">
         <v>848</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B258" s="2">
         <v>32</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D258" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E258" t="s">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1378</v>
+      </c>
+      <c r="F258" t="s">
+        <v>1392</v>
+      </c>
+      <c r="G258" t="s">
+        <v>1391</v>
+      </c>
+      <c r="H258">
+        <v>2020</v>
+      </c>
+      <c r="I258">
+        <v>1103977614</v>
+      </c>
+      <c r="J258" t="s">
+        <v>1394</v>
+      </c>
+      <c r="L258" s="2">
+        <v>1</v>
+      </c>
+      <c r="M258" t="s">
+        <v>1393</v>
+      </c>
+      <c r="N258">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="259" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B259" s="2">
         <v>32</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D259" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E259" t="s">
-        <v>1381</v>
-      </c>
-    </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1379</v>
+      </c>
+      <c r="F259" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G259" t="s">
+        <v>1396</v>
+      </c>
+      <c r="H259">
+        <v>2018</v>
+      </c>
+      <c r="I259" t="s">
+        <v>1398</v>
+      </c>
+      <c r="J259" t="s">
+        <v>1397</v>
+      </c>
+      <c r="L259" s="2">
+        <v>1</v>
+      </c>
+      <c r="M259" t="s">
+        <v>1399</v>
+      </c>
+      <c r="N259">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="260" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B260" s="2">
         <v>32</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D260" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E260" t="s">
-        <v>1382</v>
-      </c>
-    </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1380</v>
+      </c>
+      <c r="F260" t="s">
+        <v>1403</v>
+      </c>
+      <c r="G260" t="s">
+        <v>1402</v>
+      </c>
+      <c r="H260">
+        <v>2019</v>
+      </c>
+      <c r="I260">
+        <v>1126217718</v>
+      </c>
+      <c r="J260" t="s">
+        <v>1401</v>
+      </c>
+      <c r="L260" s="2">
+        <v>1</v>
+      </c>
+      <c r="M260" t="s">
+        <v>1400</v>
+      </c>
+      <c r="N260">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="261" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B261" s="2">
         <v>32</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D261" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E261" t="s">
-        <v>1383</v>
-      </c>
-    </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1381</v>
+      </c>
+      <c r="F261" t="s">
+        <v>1405</v>
+      </c>
+      <c r="G261" t="s">
+        <v>1404</v>
+      </c>
+      <c r="H261">
+        <v>2016</v>
+      </c>
+      <c r="I261">
+        <v>962391614</v>
+      </c>
+      <c r="J261" t="s">
+        <v>1407</v>
+      </c>
+      <c r="L261" s="2">
+        <v>1</v>
+      </c>
+      <c r="M261" t="s">
+        <v>1406</v>
+      </c>
+      <c r="N261">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="262" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B262" s="2">
         <v>32</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D262" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E262" t="s">
-        <v>1384</v>
-      </c>
-    </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1382</v>
+      </c>
+      <c r="F262" t="s">
+        <v>1408</v>
+      </c>
+      <c r="G262" t="s">
+        <v>1409</v>
+      </c>
+      <c r="H262">
+        <v>2008</v>
+      </c>
+      <c r="I262">
+        <v>97801410357</v>
+      </c>
+      <c r="J262" t="s">
+        <v>1410</v>
+      </c>
+      <c r="L262" s="2">
+        <v>1</v>
+      </c>
+      <c r="M262" t="s">
+        <v>1411</v>
+      </c>
+      <c r="N262">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="263" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B263" s="2">
         <v>32</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D263" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E263" t="s">
-        <v>1385</v>
-      </c>
-    </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1383</v>
+      </c>
+      <c r="F263" t="s">
+        <v>1412</v>
+      </c>
+      <c r="G263" t="s">
+        <v>1413</v>
+      </c>
+      <c r="H263">
+        <v>2020</v>
+      </c>
+      <c r="I263">
+        <v>1140369992</v>
+      </c>
+      <c r="J263" t="s">
+        <v>1414</v>
+      </c>
+      <c r="L263" s="2">
+        <v>1</v>
+      </c>
+      <c r="M263" t="s">
+        <v>1415</v>
+      </c>
+      <c r="N263">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="264" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B264" s="2">
         <v>32</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D264" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E264" t="s">
-        <v>1386</v>
-      </c>
-    </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.35">
+        <v>1384</v>
+      </c>
+      <c r="F264" t="s">
+        <v>1418</v>
+      </c>
+      <c r="G264" t="s">
+        <v>1417</v>
+      </c>
+      <c r="H264">
+        <v>2024</v>
+      </c>
+      <c r="I264">
+        <v>1412153743</v>
+      </c>
+      <c r="J264" t="s">
+        <v>1416</v>
+      </c>
+      <c r="L264" s="2">
+        <v>1</v>
+      </c>
+      <c r="M264" t="s">
+        <v>1419</v>
+      </c>
+      <c r="N264">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="265" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="B265" s="2">
         <v>32</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D265" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="E265" t="s">
-        <v>1387</v>
+        <v>1385</v>
+      </c>
+      <c r="F265" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G265" t="s">
+        <v>1422</v>
+      </c>
+      <c r="H265">
+        <v>2013</v>
+      </c>
+      <c r="I265">
+        <v>780815260</v>
+      </c>
+      <c r="J265" t="s">
+        <v>1421</v>
+      </c>
+      <c r="L265" s="2">
+        <v>1</v>
+      </c>
+      <c r="M265" t="s">
+        <v>1420</v>
+      </c>
+      <c r="N265">
+        <v>848</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:N265" xr:uid="{C17C54CB-A494-4D8A-8C6C-09250B011A75}">
-    <filterColumn colId="0">
+    <filterColumn colId="4">
       <filters>
-        <filter val="Elif Ozcan"/>
+        <filter val="Advanced Aircraft Design: Conceptual Design, Analysis and Optimization of Subsonic Civil Airplanes"/>
+        <filter val="Introduction to Transonic Aerodynamics"/>
+        <filter val="Sonic experience: a guide to everyday sounds"/>
+        <filter val="Synthesis of Subsonic Airplane Design"/>
+        <filter val="The fundamentals of sonic art &amp; sound design"/>
       </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N238">

</xml_diff>

<commit_message>
Added all covers for new recommenders. Fixed #12
</commit_message>
<xml_diff>
--- a/src/data/workshop_data/recommended_books.xlsx
+++ b/src/data/workshop_data/recommended_books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\workshop_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E305CD-8618-4111-8B8F-88E542BBA383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5FA52A-B7CD-4568-A990-C446EFBF2D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{BE54A3D7-AD18-4D3A-9B07-972BEB6CC897}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="1428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="1467">
   <si>
     <t>recommender</t>
   </si>
@@ -4231,12 +4231,6 @@
     <t>978-9082748505</t>
   </si>
   <si>
-    <t>Ben Redwood, Filemon Schöffer, Brian Garret</t>
-  </si>
-  <si>
-    <t>The 3D Printing Handbook provides actionable advice on selecting the right technology and how-to design for 3D printing, based upon first-hand experience from the industry’s leading experts. In this book: • The mechanisms behind all major 3D printing technologies • The benefits and limitations of each technology • Decision making tools for technology selection • Actionable design advice and guidelines • Industry case studies from world-leading brands</t>
-  </si>
-  <si>
     <t>978-9460031120</t>
   </si>
   <si>
@@ -4552,6 +4546,137 @@
   </si>
   <si>
     <t>839343829.webp</t>
+  </si>
+  <si>
+    <t>1362866564.webp</t>
+  </si>
+  <si>
+    <t>1378931447.webp</t>
+  </si>
+  <si>
+    <t>1354951065.webp</t>
+  </si>
+  <si>
+    <t>23972182.webp</t>
+  </si>
+  <si>
+    <t>1369522939.webp</t>
+  </si>
+  <si>
+    <t>71807799.webp</t>
+  </si>
+  <si>
+    <t>Bjarki Hallgrimsson</t>
+  </si>
+  <si>
+    <t>Ben Redwood</t>
+  </si>
+  <si>
+    <t>Neil A. Gershenfeld</t>
+  </si>
+  <si>
+    <t>Eva Hornecker, Luigina Ciolfi</t>
+  </si>
+  <si>
+    <t>Sandra H. Dudley</t>
+  </si>
+  <si>
+    <t>Kristina Höök</t>
+  </si>
+  <si>
+    <t>Andy Clark</t>
+  </si>
+  <si>
+    <t>Laura J. Snyder</t>
+  </si>
+  <si>
+    <t>978-0393077469</t>
+  </si>
+  <si>
+    <t>Snyder transports us to the streets, inns, and guildhalls of seventeenth-century Holland, where artists and scientists gathered, and to their studios and laboratories, where they mixed paints and prepared canvases, ground and polished lenses, examined and dissected insects and other animals, and invented the modern notion of seeing ... [bringing] Vermeer and Van Leeuwenhoek--and the men and women around them--vividly to life"--Dust jacket flap."The remarkable story of how an artist and a scientist in seventeenth-century Holland transformed the way we see the world. On a summer day in 1674, in the small Dutch city of Delft, Antoni van Leeuwenhoek--a cloth salesman, local bureaucrat, and self-taught natural philosopher--gazed through a tiny lens set into a brass holder and discovered a never-before imagined world of microscopic life. At the same time, in a nearby attic, the painter Johannes Vermeer was using another optical device, a camera obscura, to experiment with light and create the most luminous pictures ever beheld. "See for yourself!" was the clarion call of the 1600s. Scientists peered at nature through microscopes and telescopes, making the discoveries in astronomy, physics, chemistry, and anatomy that ignited the Scientific Revolution. Artists investigated nature with lenses, mirrors, and camera obscuras, creating extraordinarily detailed paintings of flowers and insects, and scenes filled with realistic effects of light, shadow, and color. By extending the reach of sight the new optical instruments prompted the realization that there is more than meets the eye. But they also raised questions about how we see and what it means to see. In answering these questions, scientists and artists in Delft changed how we perceive the world."--The publisher's description.</t>
+  </si>
+  <si>
+    <t>892514232.webp</t>
+  </si>
+  <si>
+    <t>Building prototypes and models is an essential component of any design activity. Prototyping and Modelmaking for Product Design illustrates how prototypes are used to help designers understand problems better, explore more imaginative solutions, investigate human interaction more fully and test functionality so as to de-risk the design process. Following an introduction on the purpose of prototyping, specific materials, tools and techniques are examined in detail, with step-by-step tutorials and industry examples of real and successful products illustrating how prototypes are used to help solve design problems. Workflow is also discussed, using a mixture of hands on and digital tools. A comprehensive modern prototyping approach is crucial to making informed design decisions, and forms a strategic part of a successful designer's toolkit.</t>
+  </si>
+  <si>
+    <t>978-1786275110</t>
+  </si>
+  <si>
+    <t>1082176473.webp</t>
+  </si>
+  <si>
+    <t>The 3D Printing Handbook provides practical advice on selecting the right technology and how-to design for 3D printing, based upon first-hand experience from the industry’s leading experts.
+In this book:
+• The mechanisms behind all major 3D printing technologies
+• The benefits and limitations of each technology
+• Decision making tools for technology selection
+• Actionable design advice and guidelines
+• Industry case studies from world-leading brands</t>
+  </si>
+  <si>
+    <t>978-0465027460</t>
+  </si>
+  <si>
+    <t>141382385.webp</t>
+  </si>
+  <si>
+    <t>A look into the future of consumer technology describes the next big step, personal fabrication, or the ability to design and manufacture products at home to personalized specifications, from consumer electronics to industrial tools.</t>
+  </si>
+  <si>
+    <t>978-1681735139</t>
+  </si>
+  <si>
+    <t>Museums have been a domain of study and design intervention for Human-Computer Interaction (HCI) for several decades. However, while resources providing overviews on the key issues in the scholarship have been produced in the fields of museum and visitor studies, no such resource as yet existed within HCI. This book fills this gap and covers key issues regarding the study and design of HCIs in museums. Through an on-site focus, the book examines how digital interactive technologies impact and shape galleries, exhibitions, and their visitors. It consolidates the body of work in HCI conducted in the heritage field and integrates it with insights from related fields and from digital heritage practice. Processes of HCI design and evaluation approaches for museums are also discussed. This book draws from the authors' extensive knowledge of case studies as well as from their own work to provide examples, reflections, and illustrations of relevant concepts and problems. This book is designed for students and early career researchers in HCI or Interaction Design, for more seasoned investigators who might approach the museum domain for the first time, and for researchers and practitioners in related fields such as heritage and museum studies or visitor studies. Designers who might wish to understand the HCI perspective on visitor-facing interactive technologies may also find this book useful.</t>
+  </si>
+  <si>
+    <t>1100026847.webp</t>
+  </si>
+  <si>
+    <t>978-0415492171</t>
+  </si>
+  <si>
+    <t>308216483.webp</t>
+  </si>
+  <si>
+    <t>This is an innovative interdisciplinary book about objects and people within museums and galleries. It addresses fundamental issues of human sensory, emotional and aesthetic experience of objects. The chapters explore ways and contexts in which things and people mutually interact, and raise questions about how objects carry meaning and feeling, the distinctions between objects and persons, particular qualities of the museum as context for person-object engagements, and the active and embodied role of the museum visitor.
+Museum Materialities is divided into three sections – Objects, Engagements and Interpretations – and includes a foreword by Susan Pearce and an afterword by Howard Morphy. It examines materiality and other perceptual and ontological qualities of objects themselves; embodied sensory and cognitive engagements – both personal and across a wider audience spread – with particular objects or object types in a museum or gallery setting; notions of aesthetics, affect and wellbeing in museum contexts; and creative and innovative artistic and museum practices that seek to illuminate or critique museum objects and interpretations.
+Phenomenological and other approaches to embodied experience in an emphatically material world are current in a number of academic areas, most particularly strands of material culture studies within anthropology and cognate disciplines. Thus far, however, there has been no concerted application of this kind of approach to museum collections and interactions with them by museum visitors, curators, artists and researchers. Bringing together essays by scholars and practitioners from a wide disciplinary and international base, Museum Materialities seeks to make just such a contribution. In so doing it makes a valuable and original addition to the literature of both material culture studies and museum studies.</t>
+  </si>
+  <si>
+    <t>1419440183.webp</t>
+  </si>
+  <si>
+    <t>Interaction design that entails a qualitative shift from a symbolic, language-oriented stance to an experiential stance that encompasses the entire design and use cycle. With the rise of ubiquitous technology, data-driven design, and the Internet of Things, our interactions and interfaces with technology are about to change dramatically, incorporating such emerging technologies as shape-changing interfaces, wearables, and movement-tracking apps. A successful interactive tool will allow the user to engage in a smooth, embodied, interaction, creating an intimate correspondence between users' actions and system response. And yet, as Kristina Höök points out, current design methods emphasize symbolic, language-oriented, and predominantly visual interactions. In Designing with the Body, Höök proposes a qualitative shift in interaction design to an experiential, felt, aesthetic stance that encompasses the entire design and use cycle. Höök calls this new approach soma design; it is a process that reincorporates body and movement into a design regime that has long privileged language and logic. Soma design offers an alternative to the aggressive, rapid design processes that dominate commercial interaction design; it allows (and requires) a slow, thoughtful process that takes into account fundamental human values. She argues that this new approach will yield better products and create healthier, more sustainable companies. Höök outlines the theory underlying soma design and describes motivations, methods, and tools. She offers examples of soma design "encounters" and an account of her own design process. She concludes with "A Soma Design Manifesto," which challenges interaction designers to "restart" their field-to focus on bodies and perception rather than reasoning and intellect.</t>
+  </si>
+  <si>
+    <t>978-0262551465</t>
+  </si>
+  <si>
+    <t>978-1524748456</t>
+  </si>
+  <si>
+    <t>A grand new vision of cognitive science that explains how our minds build the world, learn from it, and sometimes deceive themselves. For as long as we've studied the mind, we've believed that our senses determine what our mind perceives. But as our understanding of neuroscience and psychology has advanced in the last few decades, a new view has emerged that has proven to be both provocative and hugely powerful -- that the mind is not a passive observer, but an active predictor. At the core of this research is the radical reimagination of the way our brains process sensory information. Now this new school of "predictive processing" is arguing that we anticipate what we will see before we process the experience. Only then does our brain compare its prediction to the sensory information. At the forefront of this research is widely acclaimed philosopher Andy Clark, who has synthesized his revolutionary work on the predictive brain to explore its fascinating mechanics and implications. The most stunning of these is the realization that experience itself, because it is guided by prior expectation, is a kind of controlled hallucination. From the most mundane experiences to the most sublime, it is the mind that shapes most of our reality. Encountering errors in prediction helps us learn and makes us confident experts, but predictive feedback loops can also lock in conditions like chronic pain, addiction, and anxiety. A landmark study of cognitive science, The Experience Machine is a grand vision that sketches the extraordinary explanatory power of the predictive brain for our lives, health, world, and society.</t>
+  </si>
+  <si>
+    <t>1334720971.webp</t>
+  </si>
+  <si>
+    <t>979-8635379011</t>
+  </si>
+  <si>
+    <t>51NPDx7pYJL.webp</t>
+  </si>
+  <si>
+    <t>51NPDx7pYJL</t>
+  </si>
+  <si>
+    <t>This book forms a connection between both the worlds of Grasshopper® and 3D printing, explaining how to transform a design into a series of curves and paths for a 3D printer to use. It teaches how to write and create G-code directly within Grasshopper®, without the use of scripts or plug-ins, in easy format for existing Grasshopper® users to understand. Big experience using the software is not required, but skilled users will be able to take full advantage of the content.The book focused mainly on clay 3D printing, but the same logic can be applied to thermo-filament 3D printing (FDM) as well. The methods taught open up a wide range of new possibilities when 3D printing, like non-planar 3D printing or non-conventional paths for the 3D printer.</t>
+  </si>
+  <si>
+    <t>Diego Garcia Cuevas, Gianluca Pugliese</t>
   </si>
 </sst>
 </file>
@@ -4982,8 +5107,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M255" sqref="M255"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A247" sqref="A247:XFD247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5009,7 +5134,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1157</v>
@@ -5053,7 +5178,7 @@
         <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -5076,7 +5201,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -5084,8 +5209,26 @@
       <c r="E3" t="s">
         <v>437</v>
       </c>
+      <c r="F3" t="s">
+        <v>1462</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H3">
+        <v>2020</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1464</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1465</v>
+      </c>
       <c r="L3" s="2">
         <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>1463</v>
       </c>
       <c r="N3">
         <v>848</v>
@@ -5099,7 +5242,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D4" t="s">
         <v>133</v>
@@ -5140,7 +5283,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -5181,7 +5324,7 @@
         <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D6" t="s">
         <v>340</v>
@@ -5222,7 +5365,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D7" t="s">
         <v>27</v>
@@ -5263,7 +5406,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
@@ -5304,7 +5447,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -5345,7 +5488,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -5386,7 +5529,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D11" t="s">
         <v>191</v>
@@ -5427,7 +5570,7 @@
         <v>27</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D12" t="s">
         <v>111</v>
@@ -5468,7 +5611,7 @@
         <v>29</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
@@ -5476,8 +5619,26 @@
       <c r="E13" t="s">
         <v>438</v>
       </c>
+      <c r="F13" t="s">
+        <v>1458</v>
+      </c>
+      <c r="G13" t="s">
+        <v>1437</v>
+      </c>
+      <c r="H13">
+        <v>2024</v>
+      </c>
+      <c r="I13">
+        <v>1419440183</v>
+      </c>
+      <c r="J13" t="s">
+        <v>1457</v>
+      </c>
       <c r="L13" s="2">
         <v>1</v>
+      </c>
+      <c r="M13" t="s">
+        <v>1456</v>
       </c>
       <c r="N13">
         <v>848</v>
@@ -5491,7 +5652,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D14" t="s">
         <v>70</v>
@@ -5532,7 +5693,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D15" t="s">
         <v>340</v>
@@ -5573,7 +5734,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D16" t="s">
         <v>89</v>
@@ -5614,7 +5775,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
@@ -5622,8 +5783,26 @@
       <c r="E17" t="s">
         <v>439</v>
       </c>
+      <c r="F17" t="s">
+        <v>1440</v>
+      </c>
+      <c r="G17" t="s">
+        <v>1439</v>
+      </c>
+      <c r="H17">
+        <v>2015</v>
+      </c>
+      <c r="I17">
+        <v>892514232</v>
+      </c>
+      <c r="J17" t="s">
+        <v>1441</v>
+      </c>
       <c r="L17" s="2">
         <v>1</v>
+      </c>
+      <c r="M17" t="s">
+        <v>1442</v>
       </c>
       <c r="N17">
         <v>848</v>
@@ -5637,7 +5816,7 @@
         <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
@@ -5645,8 +5824,26 @@
       <c r="E18" t="s">
         <v>440</v>
       </c>
+      <c r="F18" t="s">
+        <v>1447</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1434</v>
+      </c>
+      <c r="H18">
+        <v>2005</v>
+      </c>
+      <c r="I18">
+        <v>141382385</v>
+      </c>
+      <c r="J18" t="s">
+        <v>1449</v>
+      </c>
       <c r="L18" s="2">
         <v>1</v>
+      </c>
+      <c r="M18" t="s">
+        <v>1448</v>
       </c>
       <c r="N18">
         <v>848</v>
@@ -5660,7 +5857,7 @@
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D19" t="s">
         <v>191</v>
@@ -5678,7 +5875,7 @@
         <v>2007</v>
       </c>
       <c r="I19" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="J19" t="s">
         <v>1193</v>
@@ -5687,7 +5884,7 @@
         <v>1</v>
       </c>
       <c r="M19" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="N19">
         <v>848</v>
@@ -5701,7 +5898,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D20" t="s">
         <v>340</v>
@@ -5742,7 +5939,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D21" t="s">
         <v>250</v>
@@ -5783,7 +5980,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D22" t="s">
         <v>27</v>
@@ -5824,7 +6021,7 @@
         <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -5832,8 +6029,26 @@
       <c r="E23" t="s">
         <v>441</v>
       </c>
+      <c r="F23" t="s">
+        <v>1450</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1435</v>
+      </c>
+      <c r="H23">
+        <v>2019</v>
+      </c>
+      <c r="I23">
+        <v>1100026847</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1451</v>
+      </c>
       <c r="L23" s="2">
         <v>1</v>
+      </c>
+      <c r="M23" t="s">
+        <v>1452</v>
       </c>
       <c r="N23">
         <v>848</v>
@@ -5847,7 +6062,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
@@ -5888,7 +6103,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D25" t="s">
         <v>191</v>
@@ -5929,7 +6144,7 @@
         <v>29</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -5937,8 +6152,26 @@
       <c r="E26" t="s">
         <v>442</v>
       </c>
+      <c r="F26" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1436</v>
+      </c>
+      <c r="H26">
+        <v>2010</v>
+      </c>
+      <c r="I26">
+        <v>308216483</v>
+      </c>
+      <c r="J26" t="s">
+        <v>1455</v>
+      </c>
       <c r="L26" s="2">
         <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>1454</v>
       </c>
       <c r="N26">
         <v>848</v>
@@ -5952,7 +6185,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D27" t="s">
         <v>191</v>
@@ -5993,7 +6226,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D28" t="s">
         <v>250</v>
@@ -6034,7 +6267,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -6042,8 +6275,26 @@
       <c r="E29" t="s">
         <v>443</v>
       </c>
+      <c r="F29" t="s">
+        <v>1444</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1432</v>
+      </c>
+      <c r="H29">
+        <v>2020</v>
+      </c>
+      <c r="I29">
+        <v>1082176473</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1443</v>
+      </c>
       <c r="L29" s="2">
         <v>1</v>
+      </c>
+      <c r="M29" t="s">
+        <v>1445</v>
       </c>
       <c r="N29">
         <v>848</v>
@@ -6057,7 +6308,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -6080,7 +6331,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D31" t="s">
         <v>70</v>
@@ -6121,7 +6372,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D32" t="s">
         <v>70</v>
@@ -6162,7 +6413,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -6203,7 +6454,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D34" t="s">
         <v>213</v>
@@ -6244,7 +6495,7 @@
         <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D35" t="s">
         <v>27</v>
@@ -6285,7 +6536,7 @@
         <v>23</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D36" t="s">
         <v>191</v>
@@ -6326,7 +6577,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D37" t="s">
         <v>70</v>
@@ -6359,7 +6610,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>435</v>
       </c>
@@ -6367,16 +6618,34 @@
         <v>29</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
       </c>
       <c r="E38" t="s">
-        <v>445</v>
+        <v>1322</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1323</v>
+      </c>
+      <c r="G38" t="s">
+        <v>1433</v>
+      </c>
+      <c r="H38">
+        <v>2020</v>
+      </c>
+      <c r="I38">
+        <v>1327959423</v>
+      </c>
+      <c r="J38" t="s">
+        <v>1446</v>
       </c>
       <c r="L38" s="2">
         <v>1</v>
+      </c>
+      <c r="M38" t="s">
+        <v>1336</v>
       </c>
       <c r="N38">
         <v>848</v>
@@ -6390,7 +6659,7 @@
         <v>25</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D39" t="s">
         <v>340</v>
@@ -6431,7 +6700,7 @@
         <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D40" t="s">
         <v>191</v>
@@ -6472,7 +6741,7 @@
         <v>18</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D41" t="s">
         <v>111</v>
@@ -6513,7 +6782,7 @@
         <v>24</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D42" t="s">
         <v>399</v>
@@ -6554,7 +6823,7 @@
         <v>14</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D43" t="s">
         <v>250</v>
@@ -6595,7 +6864,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D44" t="s">
         <v>191</v>
@@ -6636,7 +6905,7 @@
         <v>17</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D45" t="s">
         <v>133</v>
@@ -6677,7 +6946,7 @@
         <v>17</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D46" t="s">
         <v>133</v>
@@ -6718,7 +6987,7 @@
         <v>24</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D47" t="s">
         <v>399</v>
@@ -6759,7 +7028,7 @@
         <v>6</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
@@ -6800,7 +7069,7 @@
         <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D49" t="s">
         <v>191</v>
@@ -6841,7 +7110,7 @@
         <v>24</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D50" t="s">
         <v>399</v>
@@ -6882,7 +7151,7 @@
         <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D51" t="s">
         <v>191</v>
@@ -6923,7 +7192,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D52" t="s">
         <v>70</v>
@@ -6964,7 +7233,7 @@
         <v>21</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D53" t="s">
         <v>49</v>
@@ -7005,7 +7274,7 @@
         <v>21</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D54" t="s">
         <v>49</v>
@@ -7046,7 +7315,7 @@
         <v>5</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D55" t="s">
         <v>70</v>
@@ -7087,7 +7356,7 @@
         <v>30</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D56" t="s">
         <v>89</v>
@@ -7128,7 +7397,7 @@
         <v>23</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D57" t="s">
         <v>191</v>
@@ -7169,7 +7438,7 @@
         <v>21</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D58" t="s">
         <v>49</v>
@@ -7210,7 +7479,7 @@
         <v>27</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D59" t="s">
         <v>111</v>
@@ -7251,7 +7520,7 @@
         <v>21</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D60" t="s">
         <v>49</v>
@@ -7292,7 +7561,7 @@
         <v>6</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D61" t="s">
         <v>27</v>
@@ -7333,7 +7602,7 @@
         <v>18</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D62" t="s">
         <v>111</v>
@@ -7374,7 +7643,7 @@
         <v>19</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D63" t="s">
         <v>27</v>
@@ -7415,7 +7684,7 @@
         <v>30</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D64" t="s">
         <v>89</v>
@@ -7456,7 +7725,7 @@
         <v>5</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D65" t="s">
         <v>70</v>
@@ -7497,7 +7766,7 @@
         <v>4</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D66" t="s">
         <v>250</v>
@@ -7538,7 +7807,7 @@
         <v>27</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D67" t="s">
         <v>111</v>
@@ -7579,7 +7848,7 @@
         <v>22</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D68" t="s">
         <v>191</v>
@@ -7620,7 +7889,7 @@
         <v>18</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D69" t="s">
         <v>111</v>
@@ -7661,7 +7930,7 @@
         <v>17</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D70" t="s">
         <v>133</v>
@@ -7702,7 +7971,7 @@
         <v>22</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D71" t="s">
         <v>191</v>
@@ -7743,7 +8012,7 @@
         <v>6</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D72" t="s">
         <v>27</v>
@@ -7784,7 +8053,7 @@
         <v>17</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D73" t="s">
         <v>133</v>
@@ -7825,7 +8094,7 @@
         <v>8</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D74" t="s">
         <v>27</v>
@@ -7866,7 +8135,7 @@
         <v>24</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D75" t="s">
         <v>399</v>
@@ -7907,7 +8176,7 @@
         <v>14</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D76" t="s">
         <v>250</v>
@@ -7948,7 +8217,7 @@
         <v>21</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D77" t="s">
         <v>49</v>
@@ -7989,7 +8258,7 @@
         <v>13</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D78" t="s">
         <v>27</v>
@@ -8030,7 +8299,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D79" t="s">
         <v>191</v>
@@ -8071,7 +8340,7 @@
         <v>22</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D80" t="s">
         <v>191</v>
@@ -8112,7 +8381,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D81" t="s">
         <v>191</v>
@@ -8153,7 +8422,7 @@
         <v>2</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
@@ -8194,7 +8463,7 @@
         <v>19</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D83" t="s">
         <v>27</v>
@@ -8235,7 +8504,7 @@
         <v>3</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D84" t="s">
         <v>27</v>
@@ -8276,7 +8545,7 @@
         <v>21</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D85" t="s">
         <v>49</v>
@@ -8317,7 +8586,7 @@
         <v>13</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D86" t="s">
         <v>27</v>
@@ -8358,7 +8627,7 @@
         <v>2</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D87" t="s">
         <v>27</v>
@@ -8399,7 +8668,7 @@
         <v>3</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D88" t="s">
         <v>27</v>
@@ -8440,7 +8709,7 @@
         <v>8</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D89" t="s">
         <v>27</v>
@@ -8481,7 +8750,7 @@
         <v>3</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D90" t="s">
         <v>27</v>
@@ -8522,7 +8791,7 @@
         <v>22</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D91" t="s">
         <v>191</v>
@@ -8563,7 +8832,7 @@
         <v>6</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D92" t="s">
         <v>27</v>
@@ -8604,7 +8873,7 @@
         <v>3</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D93" t="s">
         <v>27</v>
@@ -8645,7 +8914,7 @@
         <v>27</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D94" t="s">
         <v>111</v>
@@ -8686,7 +8955,7 @@
         <v>7</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D95" t="s">
         <v>133</v>
@@ -8727,7 +8996,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D96" t="s">
         <v>27</v>
@@ -8768,7 +9037,7 @@
         <v>30</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D97" t="s">
         <v>89</v>
@@ -8809,7 +9078,7 @@
         <v>13</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D98" t="s">
         <v>27</v>
@@ -8842,7 +9111,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>378</v>
       </c>
@@ -8850,7 +9119,7 @@
         <v>20</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D99" t="s">
         <v>340</v>
@@ -8891,7 +9160,7 @@
         <v>25</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D100" t="s">
         <v>340</v>
@@ -8932,7 +9201,7 @@
         <v>4</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D101" t="s">
         <v>250</v>
@@ -8973,7 +9242,7 @@
         <v>18</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D102" t="s">
         <v>111</v>
@@ -9014,7 +9283,7 @@
         <v>17</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D103" t="s">
         <v>133</v>
@@ -9055,7 +9324,7 @@
         <v>6</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D104" t="s">
         <v>27</v>
@@ -9096,7 +9365,7 @@
         <v>20</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D105" t="s">
         <v>340</v>
@@ -9137,7 +9406,7 @@
         <v>18</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D106" t="s">
         <v>111</v>
@@ -9178,7 +9447,7 @@
         <v>23</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D107" t="s">
         <v>191</v>
@@ -9219,7 +9488,7 @@
         <v>18</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D108" t="s">
         <v>111</v>
@@ -9260,7 +9529,7 @@
         <v>8</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D109" t="s">
         <v>27</v>
@@ -9301,7 +9570,7 @@
         <v>19</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D110" t="s">
         <v>27</v>
@@ -9342,7 +9611,7 @@
         <v>30</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D111" t="s">
         <v>89</v>
@@ -9383,7 +9652,7 @@
         <v>24</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D112" t="s">
         <v>399</v>
@@ -9416,7 +9685,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>378</v>
       </c>
@@ -9424,7 +9693,7 @@
         <v>20</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D113" t="s">
         <v>340</v>
@@ -9465,7 +9734,7 @@
         <v>14</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D114" t="s">
         <v>250</v>
@@ -9506,7 +9775,7 @@
         <v>17</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D115" t="s">
         <v>133</v>
@@ -9547,7 +9816,7 @@
         <v>18</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D116" t="s">
         <v>111</v>
@@ -9588,7 +9857,7 @@
         <v>14</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D117" t="s">
         <v>250</v>
@@ -9629,7 +9898,7 @@
         <v>4</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D118" t="s">
         <v>250</v>
@@ -9670,7 +9939,7 @@
         <v>14</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D119" t="s">
         <v>250</v>
@@ -9711,7 +9980,7 @@
         <v>1</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D120" t="s">
         <v>191</v>
@@ -9752,7 +10021,7 @@
         <v>8</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D121" t="s">
         <v>27</v>
@@ -9793,7 +10062,7 @@
         <v>25</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D122" t="s">
         <v>340</v>
@@ -9834,7 +10103,7 @@
         <v>30</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D123" t="s">
         <v>89</v>
@@ -9875,7 +10144,7 @@
         <v>26</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D124" t="s">
         <v>213</v>
@@ -9916,7 +10185,7 @@
         <v>17</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D125" t="s">
         <v>133</v>
@@ -9954,7 +10223,7 @@
         <v>6</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D126" t="s">
         <v>27</v>
@@ -9995,7 +10264,7 @@
         <v>24</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D127" t="s">
         <v>399</v>
@@ -10036,7 +10305,7 @@
         <v>7</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D128" t="s">
         <v>133</v>
@@ -10077,7 +10346,7 @@
         <v>4</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D129" t="s">
         <v>250</v>
@@ -10118,7 +10387,7 @@
         <v>3</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D130" t="s">
         <v>27</v>
@@ -10159,7 +10428,7 @@
         <v>8</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D131" t="s">
         <v>27</v>
@@ -10200,7 +10469,7 @@
         <v>20</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D132" t="s">
         <v>340</v>
@@ -10241,7 +10510,7 @@
         <v>21</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D133" t="s">
         <v>49</v>
@@ -10282,7 +10551,7 @@
         <v>2</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D134" t="s">
         <v>27</v>
@@ -10323,7 +10592,7 @@
         <v>19</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D135" t="s">
         <v>27</v>
@@ -10364,7 +10633,7 @@
         <v>4</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D136" t="s">
         <v>250</v>
@@ -10405,7 +10674,7 @@
         <v>4</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D137" t="s">
         <v>250</v>
@@ -10446,7 +10715,7 @@
         <v>19</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D138" t="s">
         <v>27</v>
@@ -10487,7 +10756,7 @@
         <v>13</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D139" t="s">
         <v>27</v>
@@ -10528,7 +10797,7 @@
         <v>20</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D140" t="s">
         <v>340</v>
@@ -10569,7 +10838,7 @@
         <v>1</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D141" t="s">
         <v>191</v>
@@ -10610,7 +10879,7 @@
         <v>25</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D142" t="s">
         <v>340</v>
@@ -10651,7 +10920,7 @@
         <v>2</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D143" t="s">
         <v>27</v>
@@ -10692,7 +10961,7 @@
         <v>20</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D144" t="s">
         <v>340</v>
@@ -10733,7 +11002,7 @@
         <v>3</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D145" t="s">
         <v>27</v>
@@ -10774,7 +11043,7 @@
         <v>6</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D146" t="s">
         <v>27</v>
@@ -10807,7 +11076,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>339</v>
       </c>
@@ -10815,7 +11084,7 @@
         <v>25</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D147" t="s">
         <v>340</v>
@@ -10856,7 +11125,7 @@
         <v>4</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D148" t="s">
         <v>250</v>
@@ -10897,7 +11166,7 @@
         <v>17</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D149" t="s">
         <v>133</v>
@@ -10938,7 +11207,7 @@
         <v>26</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D150" t="s">
         <v>213</v>
@@ -10979,7 +11248,7 @@
         <v>30</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D151" t="s">
         <v>89</v>
@@ -11020,7 +11289,7 @@
         <v>23</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D152" t="s">
         <v>191</v>
@@ -11061,7 +11330,7 @@
         <v>7</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D153" t="s">
         <v>133</v>
@@ -11102,7 +11371,7 @@
         <v>19</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D154" t="s">
         <v>27</v>
@@ -11143,7 +11412,7 @@
         <v>7</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D155" t="s">
         <v>133</v>
@@ -11184,7 +11453,7 @@
         <v>26</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D156" t="s">
         <v>213</v>
@@ -11225,7 +11494,7 @@
         <v>2</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D157" t="s">
         <v>27</v>
@@ -11266,7 +11535,7 @@
         <v>19</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D158" t="s">
         <v>27</v>
@@ -11307,7 +11576,7 @@
         <v>24</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D159" t="s">
         <v>399</v>
@@ -11348,7 +11617,7 @@
         <v>26</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D160" t="s">
         <v>213</v>
@@ -11389,7 +11658,7 @@
         <v>22</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D161" t="s">
         <v>191</v>
@@ -11430,7 +11699,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D162" t="s">
         <v>191</v>
@@ -11471,7 +11740,7 @@
         <v>30</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D163" t="s">
         <v>89</v>
@@ -11512,7 +11781,7 @@
         <v>7</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D164" t="s">
         <v>133</v>
@@ -11553,7 +11822,7 @@
         <v>28</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D165" t="s">
         <v>5</v>
@@ -11594,7 +11863,7 @@
         <v>1</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D166" t="s">
         <v>191</v>
@@ -11635,7 +11904,7 @@
         <v>14</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D167" t="s">
         <v>250</v>
@@ -11676,7 +11945,7 @@
         <v>7</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D168" t="s">
         <v>133</v>
@@ -11717,7 +11986,7 @@
         <v>4</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D169" t="s">
         <v>250</v>
@@ -11758,7 +12027,7 @@
         <v>13</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D170" t="s">
         <v>27</v>
@@ -11799,7 +12068,7 @@
         <v>27</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D171" t="s">
         <v>111</v>
@@ -11840,7 +12109,7 @@
         <v>28</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D172" t="s">
         <v>5</v>
@@ -11881,7 +12150,7 @@
         <v>21</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D173" t="s">
         <v>49</v>
@@ -11922,7 +12191,7 @@
         <v>24</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D174" t="s">
         <v>399</v>
@@ -11963,7 +12232,7 @@
         <v>28</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D175" t="s">
         <v>5</v>
@@ -12004,7 +12273,7 @@
         <v>22</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D176" t="s">
         <v>191</v>
@@ -12045,7 +12314,7 @@
         <v>28</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D177" t="s">
         <v>5</v>
@@ -12086,7 +12355,7 @@
         <v>17</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D178" t="s">
         <v>133</v>
@@ -12127,7 +12396,7 @@
         <v>8</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D179" t="s">
         <v>27</v>
@@ -12168,7 +12437,7 @@
         <v>23</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D180" t="s">
         <v>191</v>
@@ -12209,7 +12478,7 @@
         <v>19</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D181" t="s">
         <v>27</v>
@@ -12250,7 +12519,7 @@
         <v>26</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D182" t="s">
         <v>213</v>
@@ -12291,7 +12560,7 @@
         <v>5</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D183" t="s">
         <v>70</v>
@@ -12332,7 +12601,7 @@
         <v>25</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D184" t="s">
         <v>340</v>
@@ -12373,7 +12642,7 @@
         <v>26</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D185" t="s">
         <v>213</v>
@@ -12414,7 +12683,7 @@
         <v>7</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D186" t="s">
         <v>133</v>
@@ -12455,7 +12724,7 @@
         <v>2</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D187" t="s">
         <v>27</v>
@@ -12496,7 +12765,7 @@
         <v>28</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D188" t="s">
         <v>5</v>
@@ -12537,7 +12806,7 @@
         <v>29</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D189" t="s">
         <v>5</v>
@@ -12578,7 +12847,7 @@
         <v>24</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D190" t="s">
         <v>399</v>
@@ -12619,7 +12888,7 @@
         <v>20</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D191" t="s">
         <v>340</v>
@@ -12660,7 +12929,7 @@
         <v>21</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D192" t="s">
         <v>49</v>
@@ -12701,7 +12970,7 @@
         <v>4</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D193" t="s">
         <v>250</v>
@@ -12742,7 +13011,7 @@
         <v>14</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D194" t="s">
         <v>250</v>
@@ -12783,7 +13052,7 @@
         <v>2</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D195" t="s">
         <v>27</v>
@@ -12824,7 +13093,7 @@
         <v>5</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D196" t="s">
         <v>70</v>
@@ -12865,7 +13134,7 @@
         <v>3</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D197" t="s">
         <v>27</v>
@@ -12906,7 +13175,7 @@
         <v>23</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D198" t="s">
         <v>191</v>
@@ -12947,7 +13216,7 @@
         <v>23</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D199" t="s">
         <v>191</v>
@@ -12988,7 +13257,7 @@
         <v>1</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D200" t="s">
         <v>191</v>
@@ -13029,7 +13298,7 @@
         <v>7</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D201" t="s">
         <v>133</v>
@@ -13070,7 +13339,7 @@
         <v>13</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D202" t="s">
         <v>27</v>
@@ -13111,7 +13380,7 @@
         <v>19</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D203" t="s">
         <v>27</v>
@@ -13152,7 +13421,7 @@
         <v>8</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D204" t="s">
         <v>27</v>
@@ -13193,7 +13462,7 @@
         <v>18</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D205" t="s">
         <v>111</v>
@@ -13234,7 +13503,7 @@
         <v>13</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D206" t="s">
         <v>27</v>
@@ -13275,7 +13544,7 @@
         <v>2</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D207" t="s">
         <v>27</v>
@@ -13316,7 +13585,7 @@
         <v>19</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>1351</v>
+        <v>1349</v>
       </c>
       <c r="D208" t="s">
         <v>27</v>
@@ -13357,7 +13626,7 @@
         <v>8</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D209" t="s">
         <v>27</v>
@@ -13398,7 +13667,7 @@
         <v>13</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D210" t="s">
         <v>27</v>
@@ -13439,7 +13708,7 @@
         <v>28</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D211" t="s">
         <v>5</v>
@@ -13480,7 +13749,7 @@
         <v>1</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D212" t="s">
         <v>191</v>
@@ -13521,7 +13790,7 @@
         <v>4</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>1346</v>
+        <v>1344</v>
       </c>
       <c r="D213" t="s">
         <v>250</v>
@@ -13562,7 +13831,7 @@
         <v>20</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D214" t="s">
         <v>340</v>
@@ -13603,7 +13872,7 @@
         <v>24</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D215" t="s">
         <v>399</v>
@@ -13644,7 +13913,7 @@
         <v>14</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D216" t="s">
         <v>250</v>
@@ -13685,7 +13954,7 @@
         <v>28</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D217" t="s">
         <v>5</v>
@@ -13726,7 +13995,7 @@
         <v>6</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D218" t="s">
         <v>27</v>
@@ -13767,7 +14036,7 @@
         <v>17</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D219" t="s">
         <v>133</v>
@@ -13808,7 +14077,7 @@
         <v>25</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D220" t="s">
         <v>340</v>
@@ -13849,7 +14118,7 @@
         <v>21</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>1350</v>
+        <v>1348</v>
       </c>
       <c r="D221" t="s">
         <v>49</v>
@@ -13890,7 +14159,7 @@
         <v>25</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D222" t="s">
         <v>340</v>
@@ -13931,7 +14200,7 @@
         <v>26</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D223" t="s">
         <v>213</v>
@@ -13972,7 +14241,7 @@
         <v>30</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D224" t="s">
         <v>89</v>
@@ -14013,7 +14282,7 @@
         <v>5</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D225" t="s">
         <v>70</v>
@@ -14054,7 +14323,7 @@
         <v>13</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D226" t="s">
         <v>27</v>
@@ -14095,7 +14364,7 @@
         <v>6</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D227" t="s">
         <v>27</v>
@@ -14136,7 +14405,7 @@
         <v>22</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>1348</v>
+        <v>1346</v>
       </c>
       <c r="D228" t="s">
         <v>191</v>
@@ -14177,7 +14446,7 @@
         <v>26</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D229" t="s">
         <v>213</v>
@@ -14218,7 +14487,7 @@
         <v>13</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D230" t="s">
         <v>27</v>
@@ -14259,7 +14528,7 @@
         <v>7</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>1344</v>
+        <v>1342</v>
       </c>
       <c r="D231" t="s">
         <v>133</v>
@@ -14297,7 +14566,7 @@
         <v>30</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D232" t="s">
         <v>89</v>
@@ -14335,7 +14604,7 @@
         <v>18</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D233" t="s">
         <v>111</v>
@@ -14376,7 +14645,7 @@
         <v>26</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D234" t="s">
         <v>213</v>
@@ -14417,7 +14686,7 @@
         <v>18</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>1347</v>
+        <v>1345</v>
       </c>
       <c r="D235" t="s">
         <v>111</v>
@@ -14458,7 +14727,7 @@
         <v>28</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D236" t="s">
         <v>5</v>
@@ -14499,7 +14768,7 @@
         <v>28</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D237" t="s">
         <v>5</v>
@@ -14540,7 +14809,7 @@
         <v>20</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>1345</v>
+        <v>1343</v>
       </c>
       <c r="D238" t="s">
         <v>340</v>
@@ -14581,7 +14850,7 @@
         <v>31</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D239" t="s">
         <v>1288</v>
@@ -14606,6 +14875,9 @@
       </c>
       <c r="L239" s="2">
         <v>1</v>
+      </c>
+      <c r="M239" s="6" t="s">
+        <v>1426</v>
       </c>
       <c r="N239">
         <v>848</v>
@@ -14619,7 +14891,7 @@
         <v>31</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D240" t="s">
         <v>1288</v>
@@ -14644,6 +14916,9 @@
       </c>
       <c r="L240" s="2">
         <v>1</v>
+      </c>
+      <c r="M240" t="s">
+        <v>1427</v>
       </c>
       <c r="N240">
         <v>848</v>
@@ -14657,7 +14932,7 @@
         <v>31</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D241" t="s">
         <v>1288</v>
@@ -14682,6 +14957,9 @@
       </c>
       <c r="L241" s="2">
         <v>1</v>
+      </c>
+      <c r="M241" s="6" t="s">
+        <v>1428</v>
       </c>
       <c r="N241">
         <v>848</v>
@@ -14695,7 +14973,7 @@
         <v>31</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D242" t="s">
         <v>1288</v>
@@ -14720,6 +14998,9 @@
       </c>
       <c r="L242" s="2">
         <v>1</v>
+      </c>
+      <c r="M242" t="s">
+        <v>1429</v>
       </c>
       <c r="N242">
         <v>848</v>
@@ -14733,7 +15014,7 @@
         <v>31</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D243" t="s">
         <v>1288</v>
@@ -14758,6 +15039,9 @@
       </c>
       <c r="L243" s="2">
         <v>1</v>
+      </c>
+      <c r="M243" t="s">
+        <v>1430</v>
       </c>
       <c r="N243">
         <v>848</v>
@@ -14771,7 +15055,7 @@
         <v>31</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D244" t="s">
         <v>1288</v>
@@ -14796,6 +15080,9 @@
       </c>
       <c r="L244" s="2">
         <v>1</v>
+      </c>
+      <c r="M244" t="s">
+        <v>1431</v>
       </c>
       <c r="N244">
         <v>848</v>
@@ -14809,7 +15096,7 @@
         <v>32</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D245" t="s">
         <v>1314</v>
@@ -14836,13 +15123,13 @@
         <v>1</v>
       </c>
       <c r="M245" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="N245">
         <v>848</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>1314</v>
       </c>
@@ -14850,7 +15137,7 @@
         <v>32</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D246" t="s">
         <v>1314</v>
@@ -14877,7 +15164,7 @@
         <v>1</v>
       </c>
       <c r="M246" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="N246">
         <v>848</v>
@@ -14885,40 +15172,40 @@
     </row>
     <row r="247" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>435</v>
+        <v>1288</v>
       </c>
       <c r="B247" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>1349</v>
+        <v>1341</v>
       </c>
       <c r="D247" t="s">
-        <v>5</v>
+        <v>1288</v>
       </c>
       <c r="E247" t="s">
-        <v>1322</v>
+        <v>1326</v>
       </c>
       <c r="F247" t="s">
-        <v>1323</v>
+        <v>1324</v>
       </c>
       <c r="G247" t="s">
-        <v>1324</v>
+        <v>1325</v>
       </c>
       <c r="H247">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="I247" s="6">
-        <v>1327959423</v>
+        <v>950569633</v>
       </c>
       <c r="J247" t="s">
-        <v>1325</v>
+        <v>1327</v>
       </c>
       <c r="L247" s="2">
         <v>1</v>
       </c>
       <c r="M247" s="3" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="N247">
         <v>848</v>
@@ -14932,7 +15219,7 @@
         <v>31</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D248" t="s">
         <v>1288</v>
@@ -14941,25 +15228,25 @@
         <v>1328</v>
       </c>
       <c r="F248" t="s">
-        <v>1326</v>
+        <v>1329</v>
       </c>
       <c r="G248" t="s">
-        <v>1327</v>
+        <v>1330</v>
       </c>
       <c r="H248">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="I248" s="6">
-        <v>950569633</v>
+        <v>1286804805</v>
       </c>
       <c r="J248" t="s">
-        <v>1329</v>
+        <v>1331</v>
       </c>
       <c r="L248" s="2">
         <v>1</v>
       </c>
       <c r="M248" s="3" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="N248">
         <v>848</v>
@@ -14973,34 +15260,34 @@
         <v>31</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D249" t="s">
         <v>1288</v>
       </c>
       <c r="E249" t="s">
-        <v>1330</v>
+        <v>1332</v>
       </c>
       <c r="F249" t="s">
-        <v>1331</v>
+        <v>1333</v>
       </c>
       <c r="G249" t="s">
-        <v>1332</v>
+        <v>1334</v>
       </c>
       <c r="H249">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="I249" s="6">
-        <v>1286804805</v>
+        <v>1452966194</v>
       </c>
       <c r="J249" t="s">
-        <v>1333</v>
+        <v>1335</v>
       </c>
       <c r="L249" s="2">
         <v>1</v>
       </c>
       <c r="M249" s="3" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="N249">
         <v>848</v>
@@ -15014,34 +15301,34 @@
         <v>31</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>1343</v>
+        <v>1341</v>
       </c>
       <c r="D250" t="s">
         <v>1288</v>
       </c>
       <c r="E250" t="s">
-        <v>1334</v>
+        <v>1350</v>
       </c>
       <c r="F250" t="s">
-        <v>1335</v>
+        <v>1352</v>
       </c>
       <c r="G250" t="s">
-        <v>1336</v>
+        <v>1351</v>
       </c>
       <c r="H250">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="I250" s="6">
-        <v>1452966194</v>
+        <v>858914389</v>
       </c>
       <c r="J250" t="s">
-        <v>1337</v>
+        <v>1353</v>
       </c>
       <c r="L250" s="2">
         <v>1</v>
       </c>
-      <c r="M250" s="3" t="s">
-        <v>1341</v>
+      <c r="M250" s="6" t="s">
+        <v>1354</v>
       </c>
       <c r="N250">
         <v>848</v>
@@ -15049,40 +15336,40 @@
     </row>
     <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>1288</v>
+        <v>1314</v>
       </c>
       <c r="B251" s="2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>1343</v>
+        <v>1347</v>
       </c>
       <c r="D251" t="s">
-        <v>1288</v>
+        <v>1314</v>
       </c>
       <c r="E251" t="s">
-        <v>1352</v>
+        <v>90</v>
       </c>
       <c r="F251" t="s">
-        <v>1354</v>
+        <v>91</v>
       </c>
       <c r="G251" t="s">
-        <v>1353</v>
+        <v>497</v>
       </c>
       <c r="H251">
-        <v>2014</v>
-      </c>
-      <c r="I251" s="6">
-        <v>858914389</v>
+        <v>2019</v>
+      </c>
+      <c r="I251" t="s">
+        <v>821</v>
       </c>
       <c r="J251" t="s">
-        <v>1355</v>
+        <v>822</v>
       </c>
       <c r="L251" s="2">
         <v>1</v>
       </c>
-      <c r="M251" s="6" t="s">
-        <v>1356</v>
+      <c r="M251" t="s">
+        <v>1262</v>
       </c>
       <c r="N251">
         <v>848</v>
@@ -15096,34 +15383,34 @@
         <v>32</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D252" t="s">
         <v>1314</v>
       </c>
       <c r="E252" t="s">
-        <v>90</v>
+        <v>1355</v>
       </c>
       <c r="F252" t="s">
-        <v>91</v>
+        <v>1357</v>
       </c>
       <c r="G252" t="s">
-        <v>497</v>
+        <v>1356</v>
       </c>
       <c r="H252">
-        <v>2019</v>
-      </c>
-      <c r="I252" t="s">
-        <v>821</v>
+        <v>2023</v>
+      </c>
+      <c r="I252">
+        <v>1379313397</v>
       </c>
       <c r="J252" t="s">
-        <v>822</v>
+        <v>1358</v>
       </c>
       <c r="L252" s="2">
         <v>1</v>
       </c>
       <c r="M252" t="s">
-        <v>1262</v>
+        <v>1359</v>
       </c>
       <c r="N252">
         <v>848</v>
@@ -15137,34 +15424,34 @@
         <v>32</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D253" t="s">
         <v>1314</v>
       </c>
       <c r="E253" t="s">
-        <v>1357</v>
+        <v>1360</v>
       </c>
       <c r="F253" t="s">
-        <v>1359</v>
+        <v>1361</v>
       </c>
       <c r="G253" t="s">
-        <v>1358</v>
+        <v>1362</v>
       </c>
       <c r="H253">
-        <v>2023</v>
+        <v>1999</v>
       </c>
       <c r="I253">
-        <v>1379313397</v>
+        <v>782888043</v>
       </c>
       <c r="J253" t="s">
-        <v>1360</v>
+        <v>1364</v>
       </c>
       <c r="L253" s="2">
         <v>1</v>
       </c>
       <c r="M253" t="s">
-        <v>1361</v>
+        <v>1363</v>
       </c>
       <c r="N253">
         <v>848</v>
@@ -15178,40 +15465,40 @@
         <v>32</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D254" t="s">
         <v>1314</v>
       </c>
       <c r="E254" t="s">
-        <v>1362</v>
+        <v>1365</v>
       </c>
       <c r="F254" t="s">
-        <v>1363</v>
+        <v>1366</v>
       </c>
       <c r="G254" t="s">
-        <v>1364</v>
+        <v>1367</v>
       </c>
       <c r="H254">
-        <v>1999</v>
+        <v>2007</v>
       </c>
       <c r="I254">
-        <v>782888043</v>
+        <v>82672512</v>
       </c>
       <c r="J254" t="s">
-        <v>1366</v>
+        <v>1369</v>
       </c>
       <c r="L254" s="2">
         <v>1</v>
       </c>
       <c r="M254" t="s">
-        <v>1365</v>
+        <v>1368</v>
       </c>
       <c r="N254">
         <v>848</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>1314</v>
       </c>
@@ -15219,34 +15506,34 @@
         <v>32</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D255" t="s">
         <v>1314</v>
       </c>
       <c r="E255" t="s">
-        <v>1367</v>
+        <v>1370</v>
       </c>
       <c r="F255" t="s">
-        <v>1368</v>
+        <v>1371</v>
       </c>
       <c r="G255" t="s">
-        <v>1369</v>
+        <v>1372</v>
       </c>
       <c r="H255">
-        <v>2007</v>
+        <v>2020</v>
       </c>
       <c r="I255">
-        <v>82672512</v>
+        <v>1086015792</v>
       </c>
       <c r="J255" t="s">
-        <v>1371</v>
+        <v>1374</v>
       </c>
       <c r="L255" s="2">
         <v>1</v>
       </c>
       <c r="M255" t="s">
-        <v>1370</v>
+        <v>1373</v>
       </c>
       <c r="N255">
         <v>848</v>
@@ -15260,34 +15547,34 @@
         <v>32</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D256" t="s">
         <v>1314</v>
       </c>
       <c r="E256" t="s">
-        <v>1372</v>
+        <v>1375</v>
       </c>
       <c r="F256" t="s">
-        <v>1373</v>
+        <v>1386</v>
       </c>
       <c r="G256" t="s">
-        <v>1374</v>
+        <v>1384</v>
       </c>
       <c r="H256">
-        <v>2020</v>
-      </c>
-      <c r="I256">
-        <v>1086015792</v>
+        <v>2023</v>
+      </c>
+      <c r="I256" t="s">
+        <v>1387</v>
       </c>
       <c r="J256" t="s">
-        <v>1376</v>
+        <v>1385</v>
       </c>
       <c r="L256" s="2">
         <v>1</v>
       </c>
       <c r="M256" t="s">
-        <v>1375</v>
+        <v>1388</v>
       </c>
       <c r="N256">
         <v>848</v>
@@ -15301,34 +15588,34 @@
         <v>32</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D257" t="s">
         <v>1314</v>
       </c>
       <c r="E257" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="F257" t="s">
-        <v>1388</v>
+        <v>1390</v>
       </c>
       <c r="G257" t="s">
-        <v>1386</v>
+        <v>1389</v>
       </c>
       <c r="H257">
-        <v>2023</v>
-      </c>
-      <c r="I257" t="s">
-        <v>1389</v>
+        <v>2020</v>
+      </c>
+      <c r="I257">
+        <v>1103977614</v>
       </c>
       <c r="J257" t="s">
-        <v>1387</v>
+        <v>1392</v>
       </c>
       <c r="L257" s="2">
         <v>1</v>
       </c>
       <c r="M257" t="s">
-        <v>1390</v>
+        <v>1391</v>
       </c>
       <c r="N257">
         <v>848</v>
@@ -15342,34 +15629,34 @@
         <v>32</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D258" t="s">
         <v>1314</v>
       </c>
       <c r="E258" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="F258" t="s">
-        <v>1392</v>
+        <v>1393</v>
       </c>
       <c r="G258" t="s">
-        <v>1391</v>
+        <v>1394</v>
       </c>
       <c r="H258">
-        <v>2020</v>
-      </c>
-      <c r="I258">
-        <v>1103977614</v>
+        <v>2018</v>
+      </c>
+      <c r="I258" t="s">
+        <v>1396</v>
       </c>
       <c r="J258" t="s">
-        <v>1394</v>
+        <v>1395</v>
       </c>
       <c r="L258" s="2">
         <v>1</v>
       </c>
       <c r="M258" t="s">
-        <v>1393</v>
+        <v>1397</v>
       </c>
       <c r="N258">
         <v>848</v>
@@ -15383,34 +15670,34 @@
         <v>32</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D259" t="s">
         <v>1314</v>
       </c>
       <c r="E259" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="F259" t="s">
-        <v>1395</v>
+        <v>1401</v>
       </c>
       <c r="G259" t="s">
-        <v>1396</v>
+        <v>1400</v>
       </c>
       <c r="H259">
-        <v>2018</v>
-      </c>
-      <c r="I259" t="s">
+        <v>2019</v>
+      </c>
+      <c r="I259">
+        <v>1126217718</v>
+      </c>
+      <c r="J259" t="s">
+        <v>1399</v>
+      </c>
+      <c r="L259" s="2">
+        <v>1</v>
+      </c>
+      <c r="M259" t="s">
         <v>1398</v>
-      </c>
-      <c r="J259" t="s">
-        <v>1397</v>
-      </c>
-      <c r="L259" s="2">
-        <v>1</v>
-      </c>
-      <c r="M259" t="s">
-        <v>1399</v>
       </c>
       <c r="N259">
         <v>848</v>
@@ -15424,13 +15711,13 @@
         <v>32</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D260" t="s">
         <v>1314</v>
       </c>
       <c r="E260" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="F260" t="s">
         <v>1403</v>
@@ -15439,19 +15726,19 @@
         <v>1402</v>
       </c>
       <c r="H260">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="I260">
-        <v>1126217718</v>
+        <v>962391614</v>
       </c>
       <c r="J260" t="s">
-        <v>1401</v>
+        <v>1405</v>
       </c>
       <c r="L260" s="2">
         <v>1</v>
       </c>
       <c r="M260" t="s">
-        <v>1400</v>
+        <v>1404</v>
       </c>
       <c r="N260">
         <v>848</v>
@@ -15465,34 +15752,34 @@
         <v>32</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D261" t="s">
         <v>1314</v>
       </c>
       <c r="E261" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="F261" t="s">
-        <v>1405</v>
+        <v>1406</v>
       </c>
       <c r="G261" t="s">
-        <v>1404</v>
+        <v>1407</v>
       </c>
       <c r="H261">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="I261">
-        <v>962391614</v>
+        <v>97801410357</v>
       </c>
       <c r="J261" t="s">
-        <v>1407</v>
+        <v>1408</v>
       </c>
       <c r="L261" s="2">
         <v>1</v>
       </c>
       <c r="M261" t="s">
-        <v>1406</v>
+        <v>1409</v>
       </c>
       <c r="N261">
         <v>848</v>
@@ -15506,34 +15793,34 @@
         <v>32</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D262" t="s">
         <v>1314</v>
       </c>
       <c r="E262" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="F262" t="s">
-        <v>1408</v>
+        <v>1410</v>
       </c>
       <c r="G262" t="s">
-        <v>1409</v>
+        <v>1411</v>
       </c>
       <c r="H262">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="I262">
-        <v>97801410357</v>
+        <v>1140369992</v>
       </c>
       <c r="J262" t="s">
-        <v>1410</v>
+        <v>1412</v>
       </c>
       <c r="L262" s="2">
         <v>1</v>
       </c>
       <c r="M262" t="s">
-        <v>1411</v>
+        <v>1413</v>
       </c>
       <c r="N262">
         <v>848</v>
@@ -15547,25 +15834,25 @@
         <v>32</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D263" t="s">
         <v>1314</v>
       </c>
       <c r="E263" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="F263" t="s">
-        <v>1412</v>
+        <v>1416</v>
       </c>
       <c r="G263" t="s">
-        <v>1413</v>
+        <v>1415</v>
       </c>
       <c r="H263">
-        <v>2020</v>
+        <v>2024</v>
       </c>
       <c r="I263">
-        <v>1140369992</v>
+        <v>1412153743</v>
       </c>
       <c r="J263" t="s">
         <v>1414</v>
@@ -15574,7 +15861,7 @@
         <v>1</v>
       </c>
       <c r="M263" t="s">
-        <v>1415</v>
+        <v>1417</v>
       </c>
       <c r="N263">
         <v>848</v>
@@ -15588,75 +15875,75 @@
         <v>32</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D264" t="s">
         <v>1314</v>
       </c>
       <c r="E264" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
       <c r="F264" t="s">
+        <v>1421</v>
+      </c>
+      <c r="G264" t="s">
+        <v>1420</v>
+      </c>
+      <c r="H264">
+        <v>2013</v>
+      </c>
+      <c r="I264">
+        <v>780815260</v>
+      </c>
+      <c r="J264" t="s">
+        <v>1419</v>
+      </c>
+      <c r="L264" s="2">
+        <v>1</v>
+      </c>
+      <c r="M264" t="s">
         <v>1418</v>
       </c>
-      <c r="G264" t="s">
-        <v>1417</v>
-      </c>
-      <c r="H264">
-        <v>2024</v>
-      </c>
-      <c r="I264">
-        <v>1412153743</v>
-      </c>
-      <c r="J264" t="s">
-        <v>1416</v>
-      </c>
-      <c r="L264" s="2">
-        <v>1</v>
-      </c>
-      <c r="M264" t="s">
-        <v>1419</v>
-      </c>
       <c r="N264">
         <v>848</v>
       </c>
     </row>
     <row r="265" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A265" t="s">
-        <v>1314</v>
+      <c r="A265" s="3" t="s">
+        <v>435</v>
       </c>
       <c r="B265" s="2">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D265" t="s">
-        <v>1314</v>
+        <v>5</v>
       </c>
       <c r="E265" t="s">
-        <v>1385</v>
+        <v>445</v>
       </c>
       <c r="F265" t="s">
-        <v>1423</v>
+        <v>1459</v>
       </c>
       <c r="G265" t="s">
-        <v>1422</v>
+        <v>1438</v>
       </c>
       <c r="H265">
-        <v>2013</v>
+        <v>2023</v>
       </c>
       <c r="I265">
-        <v>780815260</v>
+        <v>1334720971</v>
       </c>
       <c r="J265" t="s">
-        <v>1421</v>
+        <v>1460</v>
       </c>
       <c r="L265" s="2">
         <v>1</v>
       </c>
       <c r="M265" t="s">
-        <v>1420</v>
+        <v>1461</v>
       </c>
       <c r="N265">
         <v>848</v>
@@ -15666,15 +15953,11 @@
   <autoFilter ref="A1:N265" xr:uid="{C17C54CB-A494-4D8A-8C6C-09250B011A75}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Advanced Aircraft Design: Conceptual Design, Analysis and Optimization of Subsonic Civil Airplanes"/>
-        <filter val="Introduction to Transonic Aerodynamics"/>
-        <filter val="Sonic experience: a guide to everyday sounds"/>
-        <filter val="Synthesis of Subsonic Airplane Design"/>
-        <filter val="The fundamentals of sonic art &amp; sound design"/>
+        <filter val="The 3D printing handbook"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N238">
-      <sortCondition ref="M1:M238"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N265">
+      <sortCondition ref="E1:E264"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -15685,7 +15968,7 @@
     <hyperlink ref="G242" r:id="rId5" display="https://tudelft.on.worldcat.org/search?queryString=au%3D%22Essed%2C%20Philomena%22%20AND%20au%3D%221955%22&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{B51A4729-0139-4234-88FA-969F9304FE21}"/>
     <hyperlink ref="G244" r:id="rId6" display="https://tudelft.on.worldcat.org/search?queryString=au%3D%22Rand%2C%20Ayn%22&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{B7CFC170-C31E-46EB-A335-09BCADDA843B}"/>
     <hyperlink ref="E244" r:id="rId7" display="https://tudelft.on.worldcat.org/search/detail/71807799?queryString=the%20fountainhead&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{9928D475-0314-42CC-9268-6EEA844058FC}"/>
-    <hyperlink ref="G253" r:id="rId8" display="https://tudelft.on.worldcat.org/search?queryString=au%3D%22Elger%2C%20Dietmar%22&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{74CE4AEF-4228-4399-986C-37E9A5ADFD70}"/>
+    <hyperlink ref="G252" r:id="rId8" display="https://tudelft.on.worldcat.org/search?queryString=au%3D%22Elger%2C%20Dietmar%22&amp;clusterResults=false&amp;groupVariantRecords=false" xr:uid="{74CE4AEF-4228-4399-986C-37E9A5ADFD70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>

</xml_diff>

<commit_message>
Added black recommendation topic dividers
</commit_message>
<xml_diff>
--- a/src/data/workshop_data/recommended_books.xlsx
+++ b/src/data/workshop_data/recommended_books.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Revi\Desktop\Github\Twin Shelves 2\src\data\workshop_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125B3458-799C-4BA6-9F92-0B54D055A9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84FC606-F8C7-4D01-A7B1-DE8073B8DE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{BE54A3D7-AD18-4D3A-9B07-972BEB6CC897}"/>
   </bookViews>
@@ -5112,7 +5112,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17C54CB-A494-4D8A-8C6C-09250B011A75}">
   <dimension ref="A1:N266"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>